<commit_message>
Lane was empty for pro 407009 Crisp
</commit_message>
<xml_diff>
--- a/private/STATIC_DATA_1.xlsx
+++ b/private/STATIC_DATA_1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -6203,7 +6203,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF291"/>
+  <dimension ref="A1:AN291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -19308,7 +19308,7 @@
         <v>772</v>
       </c>
       <c r="H198" t="s">
-        <v>791</v>
+        <v>766</v>
       </c>
       <c r="I198" t="s">
         <v>769</v>

</xml_diff>

<commit_message>
new Browser Source added
</commit_message>
<xml_diff>
--- a/private/STATIC_DATA_1.xlsx
+++ b/private/STATIC_DATA_1.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\LolVvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CDC77D-8EC0-4F8A-8159-009E9C65FABC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4773" uniqueCount="1784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4713" uniqueCount="1786">
   <si>
     <t>nickName</t>
   </si>
@@ -5380,6 +5381,12 @@
   </si>
   <si>
     <t>minitroupax_2018.png</t>
+  </si>
+  <si>
+    <t>[231125973]</t>
+  </si>
+  <si>
+    <t>[94987702]</t>
   </si>
 </sst>
 </file>
@@ -5764,10 +5771,10 @@
   <dimension ref="A1:AN313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J177" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="R292" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P194" sqref="P194"/>
+      <selection pane="bottomRight" activeCell="AE308" sqref="AE308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25658,6 +25665,12 @@
       <c r="P308" t="s">
         <v>1758</v>
       </c>
+      <c r="S308" t="s">
+        <v>1784</v>
+      </c>
+      <c r="AE308" t="s">
+        <v>1785</v>
+      </c>
     </row>
     <row r="309" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A309" s="2"/>

</xml_diff>

<commit_message>
Social media columns added
</commit_message>
<xml_diff>
--- a/private/STATIC_DATA_1.xlsx
+++ b/private/STATIC_DATA_1.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\LolVvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA59246-4FD1-46A0-AED0-E615BF2AF3DE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +16,7 @@
     <sheet name="TEAMS" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PROS!$A$1:$AN$291</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PROS!$A$1:$AQ$308</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4713" uniqueCount="1786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4719" uniqueCount="1791">
   <si>
     <t>nickName</t>
   </si>
@@ -5387,6 +5386,21 @@
   </si>
   <si>
     <t>[27971322, 54870579,67700396]</t>
+  </si>
+  <si>
+    <t>social.twitter</t>
+  </si>
+  <si>
+    <t>social.twitch</t>
+  </si>
+  <si>
+    <t>@FroggenLoL</t>
+  </si>
+  <si>
+    <t>social.facebook</t>
+  </si>
+  <si>
+    <t>@Froggen.LoL</t>
   </si>
 </sst>
 </file>
@@ -5444,7 +5458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5454,6 +5468,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -5768,13 +5783,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN313"/>
+  <dimension ref="A1:AQ313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K101" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC122" sqref="AC122"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5806,9 +5821,12 @@
     <col min="36" max="38" width="17.42578125" hidden="1" customWidth="1"/>
     <col min="39" max="39" width="17.85546875" hidden="1" customWidth="1"/>
     <col min="40" max="40" width="18.7109375" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="15" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -5929,8 +5947,17 @@
       <c r="AN1" s="3" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO1" s="3" t="s">
+        <v>1786</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>1787</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>101001</v>
       </c>
@@ -5998,7 +6025,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>101002</v>
       </c>
@@ -6066,7 +6093,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>101003</v>
       </c>
@@ -6134,7 +6161,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>101004</v>
       </c>
@@ -6202,7 +6229,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>101005</v>
       </c>
@@ -6270,7 +6297,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>102001</v>
       </c>
@@ -6338,7 +6365,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>102002</v>
       </c>
@@ -6406,7 +6433,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>102003</v>
       </c>
@@ -6474,7 +6501,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>102004</v>
       </c>
@@ -6539,7 +6566,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>102005</v>
       </c>
@@ -6607,7 +6634,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>103001</v>
       </c>
@@ -6675,7 +6702,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>103002</v>
       </c>
@@ -6740,7 +6767,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>103003</v>
       </c>
@@ -6805,7 +6832,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>103004</v>
       </c>
@@ -6873,7 +6900,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>103005</v>
       </c>
@@ -7990,7 +8017,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>107002</v>
       </c>
@@ -8055,7 +8082,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>107003</v>
       </c>
@@ -8123,7 +8150,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>107004</v>
       </c>
@@ -8191,7 +8218,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>107005</v>
       </c>
@@ -8259,7 +8286,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>108001</v>
       </c>
@@ -8324,7 +8351,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>108002</v>
       </c>
@@ -8389,7 +8416,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>108003</v>
       </c>
@@ -8450,8 +8477,17 @@
       <c r="AE39" t="s">
         <v>1662</v>
       </c>
-    </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO39" s="7" t="s">
+        <v>1788</v>
+      </c>
+      <c r="AP39" t="s">
+        <v>42</v>
+      </c>
+      <c r="AQ39" s="7" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>108004</v>
       </c>
@@ -8516,7 +8552,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>108005</v>
       </c>
@@ -8575,7 +8611,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>108006</v>
       </c>
@@ -8637,7 +8673,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>108007</v>
       </c>
@@ -8702,7 +8738,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>108008</v>
       </c>
@@ -8767,7 +8803,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>108009</v>
       </c>
@@ -8829,7 +8865,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>109001</v>
       </c>
@@ -8897,7 +8933,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>109002</v>
       </c>
@@ -8962,7 +8998,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>109003</v>
       </c>
@@ -25688,7 +25724,7 @@
       <c r="A313" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN291" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AQ308" xr:uid="{E35BDB71-4614-43CB-874F-BBE88721387F}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
1-105 Twitter IDs added.
</commit_message>
<xml_diff>
--- a/private/STATIC_DATA_1.xlsx
+++ b/private/STATIC_DATA_1.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\LolVvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F9D23C-8237-41AC-BA2F-59ADD06D5053}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4719" uniqueCount="1791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4718" uniqueCount="1790">
   <si>
     <t>nickName</t>
   </si>
@@ -5392,9 +5393,6 @@
   </si>
   <si>
     <t>social.twitch</t>
-  </si>
-  <si>
-    <t>@FroggenLoL</t>
   </si>
   <si>
     <t>social.facebook</t>
@@ -5458,7 +5456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5469,6 +5467,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -5786,10 +5790,10 @@
   <dimension ref="A1:AQ313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AO52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="AQ79" sqref="AQ79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5821,7 +5825,7 @@
     <col min="36" max="38" width="17.42578125" hidden="1" customWidth="1"/>
     <col min="39" max="39" width="17.85546875" hidden="1" customWidth="1"/>
     <col min="40" max="40" width="18.7109375" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="15" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="17" bestFit="1" customWidth="1"/>
   </cols>
@@ -5947,14 +5951,14 @@
       <c r="AN1" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AO1" s="8" t="s">
         <v>1786</v>
       </c>
       <c r="AP1" s="3" t="s">
         <v>1787</v>
       </c>
       <c r="AQ1" s="3" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.25">
@@ -6024,6 +6028,9 @@
       <c r="AE2" t="s">
         <v>791</v>
       </c>
+      <c r="AO2" s="9">
+        <v>797258274</v>
+      </c>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -6092,6 +6099,9 @@
       <c r="AE3" t="s">
         <v>791</v>
       </c>
+      <c r="AO3" s="9">
+        <v>1571431178</v>
+      </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -6160,6 +6170,9 @@
       <c r="AE4" t="s">
         <v>791</v>
       </c>
+      <c r="AO4" s="9">
+        <v>1029142980</v>
+      </c>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -6228,6 +6241,9 @@
       <c r="AE5" t="s">
         <v>791</v>
       </c>
+      <c r="AO5" s="9">
+        <v>344538810</v>
+      </c>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -6296,6 +6312,9 @@
       <c r="AE6" t="s">
         <v>791</v>
       </c>
+      <c r="AO6" s="9">
+        <v>2967174322</v>
+      </c>
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -6364,6 +6383,9 @@
       <c r="AE7" t="s">
         <v>791</v>
       </c>
+      <c r="AO7" s="9">
+        <v>8.0708557438532403E+17</v>
+      </c>
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -6432,6 +6454,9 @@
       <c r="AE8" t="s">
         <v>791</v>
       </c>
+      <c r="AO8" s="9">
+        <v>627395451</v>
+      </c>
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -6500,6 +6525,9 @@
       <c r="AE9" t="s">
         <v>791</v>
       </c>
+      <c r="AO9" s="9">
+        <v>409736208</v>
+      </c>
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -6565,6 +6593,9 @@
       <c r="AE10" t="s">
         <v>791</v>
       </c>
+      <c r="AO10" s="9">
+        <v>1891679210</v>
+      </c>
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -6633,6 +6664,9 @@
       <c r="AE11" t="s">
         <v>791</v>
       </c>
+      <c r="AO11" s="10">
+        <v>2358219158</v>
+      </c>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -6701,6 +6735,9 @@
       <c r="AE12" t="s">
         <v>791</v>
       </c>
+      <c r="AO12" s="9">
+        <v>606721954</v>
+      </c>
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -6766,6 +6803,9 @@
       <c r="AE13" t="s">
         <v>791</v>
       </c>
+      <c r="AO13" s="9">
+        <v>7.9656035538429901E+17</v>
+      </c>
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -6831,6 +6871,9 @@
       <c r="AE14" t="s">
         <v>791</v>
       </c>
+      <c r="AO14" s="9">
+        <v>2842441900</v>
+      </c>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -6899,6 +6942,9 @@
       <c r="AE15" t="s">
         <v>791</v>
       </c>
+      <c r="AO15" s="9">
+        <v>1549711460</v>
+      </c>
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -6967,8 +7013,11 @@
       <c r="AE16" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO16" s="9">
+        <v>453175900</v>
+      </c>
+    </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>104001</v>
       </c>
@@ -7035,8 +7084,11 @@
       <c r="AE17" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO17" s="9">
+        <v>2963716081</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>104002</v>
       </c>
@@ -7100,8 +7152,11 @@
       <c r="AE18" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO18" s="9">
+        <v>911330070</v>
+      </c>
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>104003</v>
       </c>
@@ -7168,8 +7223,11 @@
       <c r="AE19" t="s">
         <v>833</v>
       </c>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO19" s="9">
+        <v>2431173637</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>104004</v>
       </c>
@@ -7236,8 +7294,11 @@
       <c r="AE20" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO20" s="9">
+        <v>70681150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>104005</v>
       </c>
@@ -7304,8 +7365,11 @@
       <c r="AE21" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO21" s="9">
+        <v>2562577436</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>105001</v>
       </c>
@@ -7372,8 +7436,11 @@
       <c r="AE22" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO22" s="9">
+        <v>3033743029</v>
+      </c>
+    </row>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>105002</v>
       </c>
@@ -7437,8 +7504,11 @@
       <c r="AE23" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO23" s="9">
+        <v>3240335132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>105003</v>
       </c>
@@ -7502,8 +7572,11 @@
       <c r="AE24" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO24" s="9">
+        <v>2355746030</v>
+      </c>
+    </row>
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>105004</v>
       </c>
@@ -7570,8 +7643,11 @@
       <c r="AE25" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO25" s="9">
+        <v>555641003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>105005</v>
       </c>
@@ -7635,8 +7711,11 @@
       <c r="AE26" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO26" s="9">
+        <v>1312663430</v>
+      </c>
+    </row>
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>106001</v>
       </c>
@@ -7694,8 +7773,11 @@
       <c r="AE27" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO27" s="9">
+        <v>3219379807</v>
+      </c>
+    </row>
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>106002</v>
       </c>
@@ -7762,8 +7844,11 @@
       <c r="AE28" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO28" s="9">
+        <v>7.3076120301053504E+17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>106003</v>
       </c>
@@ -7827,8 +7912,11 @@
       <c r="AE29" t="s">
         <v>1664</v>
       </c>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO29" s="9">
+        <v>366839886</v>
+      </c>
+    </row>
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>106004</v>
       </c>
@@ -7892,8 +7980,11 @@
       <c r="AE30" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO30" s="9">
+        <v>1695450060</v>
+      </c>
+    </row>
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>106005</v>
       </c>
@@ -7957,8 +8048,11 @@
       <c r="AE31" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO31" s="9">
+        <v>2402529038</v>
+      </c>
+    </row>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>107001</v>
       </c>
@@ -8015,6 +8109,9 @@
       </c>
       <c r="AE32" t="s">
         <v>791</v>
+      </c>
+      <c r="AO32" s="9">
+        <v>550041386</v>
       </c>
     </row>
     <row r="33" spans="1:43" x14ac:dyDescent="0.25">
@@ -8081,6 +8178,9 @@
       <c r="AE33" t="s">
         <v>791</v>
       </c>
+      <c r="AO33" s="9">
+        <v>3098400658</v>
+      </c>
     </row>
     <row r="34" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
@@ -8149,6 +8249,9 @@
       <c r="AE34" t="s">
         <v>791</v>
       </c>
+      <c r="AO34" s="9">
+        <v>710300755</v>
+      </c>
     </row>
     <row r="35" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
@@ -8217,6 +8320,9 @@
       <c r="AE35" t="s">
         <v>791</v>
       </c>
+      <c r="AO35" s="9">
+        <v>1158468355</v>
+      </c>
     </row>
     <row r="36" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
@@ -8285,6 +8391,9 @@
       <c r="AE36" t="s">
         <v>791</v>
       </c>
+      <c r="AO36" s="9">
+        <v>1158473077</v>
+      </c>
     </row>
     <row r="37" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
@@ -8415,6 +8524,9 @@
       <c r="AE38" t="s">
         <v>791</v>
       </c>
+      <c r="AO38" s="9">
+        <v>2500157576</v>
+      </c>
     </row>
     <row r="39" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
@@ -8477,14 +8589,14 @@
       <c r="AE39" t="s">
         <v>1662</v>
       </c>
-      <c r="AO39" s="7" t="s">
-        <v>1788</v>
+      <c r="AO39" s="11">
+        <v>803776063</v>
       </c>
       <c r="AP39" t="s">
         <v>42</v>
       </c>
       <c r="AQ39" s="7" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="40" spans="1:43" x14ac:dyDescent="0.25">
@@ -8551,6 +8663,9 @@
       <c r="AE40" t="s">
         <v>791</v>
       </c>
+      <c r="AO40" s="9">
+        <v>1323579721</v>
+      </c>
     </row>
     <row r="41" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
@@ -8610,6 +8725,9 @@
       <c r="AE41" t="s">
         <v>791</v>
       </c>
+      <c r="AO41" s="9">
+        <v>1518796441</v>
+      </c>
     </row>
     <row r="42" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
@@ -8672,6 +8790,9 @@
       <c r="AE42" t="s">
         <v>791</v>
       </c>
+      <c r="AO42" s="9">
+        <v>8.0453309903590605E+17</v>
+      </c>
     </row>
     <row r="43" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
@@ -8737,6 +8858,9 @@
       <c r="AE43" t="s">
         <v>791</v>
       </c>
+      <c r="AO43" s="9">
+        <v>3318645734</v>
+      </c>
     </row>
     <row r="44" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
@@ -8802,6 +8926,9 @@
       <c r="AE44" t="s">
         <v>791</v>
       </c>
+      <c r="AO44" s="9">
+        <v>2881291357</v>
+      </c>
     </row>
     <row r="45" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
@@ -8864,6 +8991,9 @@
       <c r="AE45" t="s">
         <v>791</v>
       </c>
+      <c r="AO45" s="9">
+        <v>361075874</v>
+      </c>
     </row>
     <row r="46" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
@@ -8932,6 +9062,9 @@
       <c r="AE46" t="s">
         <v>791</v>
       </c>
+      <c r="AO46" s="9">
+        <v>521104742</v>
+      </c>
     </row>
     <row r="47" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
@@ -8997,6 +9130,9 @@
       <c r="AE47" t="s">
         <v>791</v>
       </c>
+      <c r="AO47" s="9">
+        <v>3333845799</v>
+      </c>
     </row>
     <row r="48" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
@@ -9065,8 +9201,11 @@
       <c r="AE48" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO48" s="9">
+        <v>8.8955887377375206E+17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>109004</v>
       </c>
@@ -9133,8 +9272,11 @@
       <c r="AE49" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO49" s="9">
+        <v>2884184449</v>
+      </c>
+    </row>
+    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>109005</v>
       </c>
@@ -9198,8 +9340,11 @@
       <c r="AE50" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO50" s="9">
+        <v>2802746749</v>
+      </c>
+    </row>
+    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>110001</v>
       </c>
@@ -9263,8 +9408,11 @@
       <c r="AE51" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO51" s="9">
+        <v>115542264</v>
+      </c>
+    </row>
+    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>110002</v>
       </c>
@@ -9328,8 +9476,11 @@
       <c r="AE52" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO52" s="9">
+        <v>8.3788326869967206E+17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>110003</v>
       </c>
@@ -9396,8 +9547,11 @@
       <c r="AE53" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO53" s="9">
+        <v>2870393113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>110004</v>
       </c>
@@ -9464,8 +9618,11 @@
       <c r="AE54" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO54" s="9">
+        <v>3180805950</v>
+      </c>
+    </row>
+    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>110005</v>
       </c>
@@ -9532,8 +9689,11 @@
       <c r="AE55" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO55" s="9">
+        <v>438136706</v>
+      </c>
+    </row>
+    <row r="56" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>201001</v>
       </c>
@@ -9600,8 +9760,11 @@
       <c r="AE56" t="s">
         <v>897</v>
       </c>
-    </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO56" s="9">
+        <v>498051521</v>
+      </c>
+    </row>
+    <row r="57" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>201002</v>
       </c>
@@ -9668,8 +9831,11 @@
       <c r="AE57" t="s">
         <v>899</v>
       </c>
-    </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO57" s="9">
+        <v>4910628093</v>
+      </c>
+    </row>
+    <row r="58" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>201003</v>
       </c>
@@ -9736,8 +9902,11 @@
       <c r="AE58" t="s">
         <v>1633</v>
       </c>
-    </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO58" s="9">
+        <v>2996912843</v>
+      </c>
+    </row>
+    <row r="59" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>201004</v>
       </c>
@@ -9804,8 +9973,11 @@
       <c r="AE59" t="s">
         <v>902</v>
       </c>
-    </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO59" s="9">
+        <v>881827464</v>
+      </c>
+    </row>
+    <row r="60" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>201005</v>
       </c>
@@ -9872,8 +10044,11 @@
       <c r="AE60" t="s">
         <v>904</v>
       </c>
-    </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO60" s="9">
+        <v>2180891672</v>
+      </c>
+    </row>
+    <row r="61" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>202001</v>
       </c>
@@ -9931,8 +10106,11 @@
       <c r="AE61" t="s">
         <v>906</v>
       </c>
-    </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO61" s="9">
+        <v>7.3226846807500301E+17</v>
+      </c>
+    </row>
+    <row r="62" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>202002</v>
       </c>
@@ -9999,8 +10177,11 @@
       <c r="AE62" t="s">
         <v>909</v>
       </c>
-    </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO62" s="9">
+        <v>189438124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>202003</v>
       </c>
@@ -10067,8 +10248,11 @@
       <c r="AE63" t="s">
         <v>911</v>
       </c>
-    </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO63" s="9">
+        <v>1648029396</v>
+      </c>
+    </row>
+    <row r="64" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>202004</v>
       </c>
@@ -10135,8 +10319,11 @@
       <c r="AE64" t="s">
         <v>914</v>
       </c>
-    </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AO64" s="9">
+        <v>1887874465</v>
+      </c>
+    </row>
+    <row r="65" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>202005</v>
       </c>
@@ -10203,8 +10390,11 @@
       <c r="AE65" t="s">
         <v>917</v>
       </c>
-    </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AO65" s="9">
+        <v>1244508066</v>
+      </c>
+    </row>
+    <row r="66" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>203001</v>
       </c>
@@ -10268,8 +10458,11 @@
       <c r="AE66" t="s">
         <v>919</v>
       </c>
-    </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AO66" s="9">
+        <v>2790180781</v>
+      </c>
+    </row>
+    <row r="67" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>203002</v>
       </c>
@@ -10336,8 +10529,11 @@
       <c r="AE67" t="s">
         <v>921</v>
       </c>
-    </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AO67" s="9">
+        <v>2893607283</v>
+      </c>
+    </row>
+    <row r="68" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>203003</v>
       </c>
@@ -10404,8 +10600,11 @@
       <c r="AE68" t="s">
         <v>923</v>
       </c>
-    </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AO68" s="9">
+        <v>2550298718</v>
+      </c>
+    </row>
+    <row r="69" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>203004</v>
       </c>
@@ -10472,8 +10671,11 @@
       <c r="AE69" t="s">
         <v>925</v>
       </c>
-    </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AO69" s="9">
+        <v>2460445795</v>
+      </c>
+    </row>
+    <row r="70" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>203005</v>
       </c>
@@ -10540,8 +10742,11 @@
       <c r="AE70" t="s">
         <v>928</v>
       </c>
-    </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AO70" s="9">
+        <v>3220569488</v>
+      </c>
+    </row>
+    <row r="71" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>204001</v>
       </c>
@@ -10599,8 +10804,11 @@
       <c r="AE71" t="s">
         <v>930</v>
       </c>
-    </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AO71" s="9">
+        <v>2262186933</v>
+      </c>
+    </row>
+    <row r="72" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>204002</v>
       </c>
@@ -10664,8 +10872,11 @@
       <c r="AE72" t="s">
         <v>932</v>
       </c>
-    </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AO72" s="9">
+        <v>3376068993</v>
+      </c>
+    </row>
+    <row r="73" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>204003</v>
       </c>
@@ -10732,8 +10943,11 @@
       <c r="AE73" t="s">
         <v>934</v>
       </c>
-    </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AO73" s="9">
+        <v>2943089668</v>
+      </c>
+    </row>
+    <row r="74" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>204004</v>
       </c>
@@ -10797,8 +11011,11 @@
       <c r="AE74" t="s">
         <v>1638</v>
       </c>
-    </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AO74" s="9">
+        <v>2275242200</v>
+      </c>
+    </row>
+    <row r="75" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>204005</v>
       </c>
@@ -10865,8 +11082,11 @@
       <c r="AE75" t="s">
         <v>1636</v>
       </c>
-    </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AO75" s="9">
+        <v>8.0530607732347597E+17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>205001</v>
       </c>
@@ -10930,8 +11150,11 @@
       <c r="AE76" t="s">
         <v>1652</v>
       </c>
-    </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AO76" s="9">
+        <v>2274984734</v>
+      </c>
+    </row>
+    <row r="77" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>205002</v>
       </c>
@@ -11004,8 +11227,11 @@
       <c r="AF77" t="s">
         <v>1628</v>
       </c>
-    </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AO77" s="9">
+        <v>2216500400</v>
+      </c>
+    </row>
+    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>205003</v>
       </c>
@@ -11072,8 +11298,11 @@
       <c r="AE78" t="s">
         <v>937</v>
       </c>
-    </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AO78" s="9">
+        <v>1974332792</v>
+      </c>
+    </row>
+    <row r="79" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>205004</v>
       </c>
@@ -11134,8 +11363,11 @@
       <c r="AE79" t="s">
         <v>939</v>
       </c>
-    </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AO79" s="9">
+        <v>8.0884771753120499E+17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>205005</v>
       </c>
@@ -11196,8 +11428,11 @@
       <c r="AE80" t="s">
         <v>941</v>
       </c>
-    </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO80" s="9">
+        <v>3290808800</v>
+      </c>
+    </row>
+    <row r="81" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>206001</v>
       </c>
@@ -11264,8 +11499,11 @@
       <c r="AE81" t="s">
         <v>943</v>
       </c>
-    </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO81" s="9">
+        <v>2776080715</v>
+      </c>
+    </row>
+    <row r="82" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>206002</v>
       </c>
@@ -11332,8 +11570,11 @@
       <c r="AE82" t="s">
         <v>945</v>
       </c>
-    </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO82" s="9">
+        <v>2767545127</v>
+      </c>
+    </row>
+    <row r="83" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>206003</v>
       </c>
@@ -11400,8 +11641,11 @@
       <c r="AE83" t="s">
         <v>947</v>
       </c>
-    </row>
-    <row r="84" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO83" s="9">
+        <v>2303751344</v>
+      </c>
+    </row>
+    <row r="84" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>206004</v>
       </c>
@@ -11465,8 +11709,11 @@
       <c r="AE84" t="s">
         <v>949</v>
       </c>
-    </row>
-    <row r="85" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO84" s="9">
+        <v>710556630</v>
+      </c>
+    </row>
+    <row r="85" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>206005</v>
       </c>
@@ -11533,8 +11780,11 @@
       <c r="AE85" t="s">
         <v>951</v>
       </c>
-    </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO85" s="9">
+        <v>2984116738</v>
+      </c>
+    </row>
+    <row r="86" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>207001</v>
       </c>
@@ -11601,8 +11851,11 @@
       <c r="AE86" t="s">
         <v>953</v>
       </c>
-    </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO86" s="9">
+        <v>2590218632</v>
+      </c>
+    </row>
+    <row r="87" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>207002</v>
       </c>
@@ -11666,8 +11919,11 @@
       <c r="AE87" t="s">
         <v>955</v>
       </c>
-    </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO87" s="9">
+        <v>1076882574</v>
+      </c>
+    </row>
+    <row r="88" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>207003</v>
       </c>
@@ -11734,8 +11990,11 @@
       <c r="AE88" t="s">
         <v>957</v>
       </c>
-    </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO88" s="9">
+        <v>1048780687</v>
+      </c>
+    </row>
+    <row r="89" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>207004</v>
       </c>
@@ -11802,8 +12061,11 @@
       <c r="AE89" t="s">
         <v>959</v>
       </c>
-    </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO89" s="9">
+        <v>1250062656</v>
+      </c>
+    </row>
+    <row r="90" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>207005</v>
       </c>
@@ -11867,8 +12129,11 @@
       <c r="AE90" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO90" s="9">
+        <v>497329859</v>
+      </c>
+    </row>
+    <row r="91" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>208001</v>
       </c>
@@ -11935,8 +12200,11 @@
       <c r="AE91" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO91" s="9">
+        <v>2685541393</v>
+      </c>
+    </row>
+    <row r="92" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>208002</v>
       </c>
@@ -12003,8 +12271,11 @@
       <c r="AE92" t="s">
         <v>1635</v>
       </c>
-    </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO92" s="9">
+        <v>3044903147</v>
+      </c>
+    </row>
+    <row r="93" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>208003</v>
       </c>
@@ -12068,8 +12339,11 @@
       <c r="AE93" t="s">
         <v>965</v>
       </c>
-    </row>
-    <row r="94" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO93" s="9">
+        <v>1648682035</v>
+      </c>
+    </row>
+    <row r="94" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>208004</v>
       </c>
@@ -12136,8 +12410,11 @@
       <c r="AE94" t="s">
         <v>967</v>
       </c>
-    </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO94" s="9">
+        <v>336118770</v>
+      </c>
+    </row>
+    <row r="95" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>208005</v>
       </c>
@@ -12204,8 +12481,11 @@
       <c r="AE95" t="s">
         <v>969</v>
       </c>
-    </row>
-    <row r="96" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO95" s="9">
+        <v>2216379312</v>
+      </c>
+    </row>
+    <row r="96" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>209001</v>
       </c>
@@ -12272,8 +12552,11 @@
       <c r="AE96" t="s">
         <v>971</v>
       </c>
-    </row>
-    <row r="97" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO96" s="9">
+        <v>2493571052</v>
+      </c>
+    </row>
+    <row r="97" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>209002</v>
       </c>
@@ -12337,8 +12620,11 @@
       <c r="AE97" t="s">
         <v>973</v>
       </c>
-    </row>
-    <row r="98" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO97" s="9">
+        <v>3199462954</v>
+      </c>
+    </row>
+    <row r="98" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>209003</v>
       </c>
@@ -12402,8 +12688,11 @@
       <c r="AE98" t="s">
         <v>975</v>
       </c>
-    </row>
-    <row r="99" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO98" s="9">
+        <v>3300282393</v>
+      </c>
+    </row>
+    <row r="99" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>209004</v>
       </c>
@@ -12467,8 +12756,11 @@
       <c r="AE99" t="s">
         <v>977</v>
       </c>
-    </row>
-    <row r="100" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO99" s="9">
+        <v>2902700080</v>
+      </c>
+    </row>
+    <row r="100" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>209005</v>
       </c>
@@ -12532,8 +12824,11 @@
       <c r="AE100" t="s">
         <v>979</v>
       </c>
-    </row>
-    <row r="101" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO100" s="9">
+        <v>2387061402</v>
+      </c>
+    </row>
+    <row r="101" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>210001</v>
       </c>
@@ -12597,8 +12892,11 @@
       <c r="AE101" t="s">
         <v>981</v>
       </c>
-    </row>
-    <row r="102" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO101" s="9">
+        <v>2199018126</v>
+      </c>
+    </row>
+    <row r="102" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>210002</v>
       </c>
@@ -12665,8 +12963,11 @@
       <c r="AE102" t="s">
         <v>983</v>
       </c>
-    </row>
-    <row r="103" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO102" s="9">
+        <v>2494302799</v>
+      </c>
+    </row>
+    <row r="103" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>210003</v>
       </c>
@@ -12730,8 +13031,11 @@
       <c r="AE103" t="s">
         <v>985</v>
       </c>
-    </row>
-    <row r="104" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO103" s="9">
+        <v>7.0327568849371098E+17</v>
+      </c>
+    </row>
+    <row r="104" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>210004</v>
       </c>
@@ -12795,8 +13099,11 @@
       <c r="AE104" t="s">
         <v>987</v>
       </c>
-    </row>
-    <row r="105" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO104" s="9">
+        <v>2387536795</v>
+      </c>
+    </row>
+    <row r="105" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>210005</v>
       </c>
@@ -12860,8 +13167,11 @@
       <c r="AE105" t="s">
         <v>989</v>
       </c>
-    </row>
-    <row r="106" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AO105" s="9">
+        <v>7.6598950418438502E+17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>301001</v>
       </c>
@@ -12926,7 +13236,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="107" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>301002</v>
       </c>
@@ -12991,7 +13301,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="108" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>301003</v>
       </c>
@@ -13059,7 +13369,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="109" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>301004</v>
       </c>
@@ -13127,7 +13437,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="110" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>301005</v>
       </c>
@@ -13195,7 +13505,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="111" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>302001</v>
       </c>
@@ -13263,7 +13573,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="112" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>302002</v>
       </c>

</xml_diff>

<commit_message>
social.twitter converted to text
</commit_message>
<xml_diff>
--- a/private/STATIC_DATA_1.xlsx
+++ b/private/STATIC_DATA_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\LolVvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0233C0C3-B08B-45DE-BC1E-C4D916DFD7F4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EA2F39-498F-42F2-9A30-B8000476C9D6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5527,12 +5527,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -5850,10 +5850,10 @@
   <dimension ref="A1:AQ313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AE262" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AF286" sqref="AF286"/>
+      <selection pane="bottomRight" activeCell="AO1" sqref="AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6443,7 +6443,7 @@
       <c r="AE7" t="s">
         <v>789</v>
       </c>
-      <c r="AO7" s="11" t="s">
+      <c r="AO7" s="10" t="s">
         <v>1791</v>
       </c>
     </row>
@@ -6724,7 +6724,7 @@
       <c r="AE11" t="s">
         <v>789</v>
       </c>
-      <c r="AO11" s="10">
+      <c r="AO11" s="11">
         <v>2358219158</v>
       </c>
     </row>
@@ -6863,7 +6863,7 @@
       <c r="AE13" t="s">
         <v>789</v>
       </c>
-      <c r="AO13" s="11" t="s">
+      <c r="AO13" s="10" t="s">
         <v>1792</v>
       </c>
     </row>
@@ -7904,7 +7904,7 @@
       <c r="AE28" t="s">
         <v>789</v>
       </c>
-      <c r="AO28" s="11" t="s">
+      <c r="AO28" s="10" t="s">
         <v>1793</v>
       </c>
     </row>
@@ -8649,7 +8649,7 @@
       <c r="AE39" t="s">
         <v>1658</v>
       </c>
-      <c r="AO39" s="11">
+      <c r="AO39" s="10">
         <v>803776063</v>
       </c>
       <c r="AP39" t="s">
@@ -9258,7 +9258,7 @@
       <c r="AE48" t="s">
         <v>789</v>
       </c>
-      <c r="AO48" s="11" t="s">
+      <c r="AO48" s="10" t="s">
         <v>1794</v>
       </c>
     </row>
@@ -9533,7 +9533,7 @@
       <c r="AE52" t="s">
         <v>789</v>
       </c>
-      <c r="AO52" s="11" t="s">
+      <c r="AO52" s="10" t="s">
         <v>1795</v>
       </c>
     </row>
@@ -10163,7 +10163,7 @@
       <c r="AE61" t="s">
         <v>904</v>
       </c>
-      <c r="AO61" s="11" t="s">
+      <c r="AO61" s="10" t="s">
         <v>1796</v>
       </c>
     </row>
@@ -11139,7 +11139,7 @@
       <c r="AE75" t="s">
         <v>1632</v>
       </c>
-      <c r="AO75" s="11" t="s">
+      <c r="AO75" s="10" t="s">
         <v>1797</v>
       </c>
     </row>
@@ -11420,7 +11420,7 @@
       <c r="AE79" t="s">
         <v>937</v>
       </c>
-      <c r="AO79" s="11" t="s">
+      <c r="AO79" s="10" t="s">
         <v>1798</v>
       </c>
     </row>
@@ -13088,7 +13088,7 @@
       <c r="AE103" t="s">
         <v>983</v>
       </c>
-      <c r="AO103" s="11" t="s">
+      <c r="AO103" s="10" t="s">
         <v>1799</v>
       </c>
     </row>
@@ -13224,7 +13224,7 @@
       <c r="AE105" t="s">
         <v>987</v>
       </c>
-      <c r="AO105" s="11" t="s">
+      <c r="AO105" s="10" t="s">
         <v>1800</v>
       </c>
     </row>
@@ -13425,7 +13425,7 @@
       <c r="AE108" t="s">
         <v>789</v>
       </c>
-      <c r="AO108" s="11" t="s">
+      <c r="AO108" s="10" t="s">
         <v>1801</v>
       </c>
     </row>
@@ -14188,7 +14188,7 @@
       <c r="AE119" t="s">
         <v>789</v>
       </c>
-      <c r="AO119" s="11" t="s">
+      <c r="AO119" s="10" t="s">
         <v>1802</v>
       </c>
     </row>
@@ -14611,7 +14611,7 @@
       <c r="AE125" t="s">
         <v>789</v>
       </c>
-      <c r="AO125" s="11" t="s">
+      <c r="AO125" s="10" t="s">
         <v>1803</v>
       </c>
     </row>
@@ -15610,7 +15610,7 @@
       <c r="AE140" t="s">
         <v>789</v>
       </c>
-      <c r="AO140" s="11" t="s">
+      <c r="AO140" s="10" t="s">
         <v>1804</v>
       </c>
     </row>
@@ -22343,7 +22343,7 @@
       <c r="AE244" t="s">
         <v>789</v>
       </c>
-      <c r="AO244" s="11" t="s">
+      <c r="AO244" s="10" t="s">
         <v>1805</v>
       </c>
     </row>
@@ -23031,7 +23031,7 @@
       <c r="AE255" t="s">
         <v>789</v>
       </c>
-      <c r="AO255" s="11" t="s">
+      <c r="AO255" s="10" t="s">
         <v>1806</v>
       </c>
     </row>
@@ -23840,7 +23840,7 @@
       <c r="AE268" t="s">
         <v>1766</v>
       </c>
-      <c r="AO268" s="11" t="s">
+      <c r="AO268" s="10" t="s">
         <v>1807</v>
       </c>
     </row>
@@ -23902,7 +23902,7 @@
       <c r="AE269" t="s">
         <v>789</v>
       </c>
-      <c r="AO269" s="11" t="s">
+      <c r="AO269" s="10" t="s">
         <v>1808</v>
       </c>
     </row>
@@ -24224,7 +24224,7 @@
       <c r="AE274" t="s">
         <v>789</v>
       </c>
-      <c r="AO274" s="11" t="s">
+      <c r="AO274" s="10" t="s">
         <v>1809</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update pro list, bwipo added
</commit_message>
<xml_diff>
--- a/private/STATIC_DATA_1.xlsx
+++ b/private/STATIC_DATA_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\LolVvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1A2228-320A-46C7-8136-B50429388747}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D092DD-8A05-4FD7-8FCA-6314F275E3E7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4737" uniqueCount="1818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4750" uniqueCount="1833">
   <si>
     <t>nickName</t>
   </si>
@@ -5483,6 +5483,51 @@
   </si>
   <si>
     <t>[69930167]</t>
+  </si>
+  <si>
+    <t>[240064189]</t>
+  </si>
+  <si>
+    <t>[107957152]</t>
+  </si>
+  <si>
+    <t>[240064544]</t>
+  </si>
+  <si>
+    <t>[107987185]</t>
+  </si>
+  <si>
+    <t>[107977099]</t>
+  </si>
+  <si>
+    <t>[240063985]</t>
+  </si>
+  <si>
+    <t>[238221594]</t>
+  </si>
+  <si>
+    <t>[106006814]</t>
+  </si>
+  <si>
+    <t>Bwipo</t>
+  </si>
+  <si>
+    <t>Gabriël </t>
+  </si>
+  <si>
+    <t>Rau</t>
+  </si>
+  <si>
+    <t>bwipo_2018.png</t>
+  </si>
+  <si>
+    <t>[38937944,37841420]</t>
+  </si>
+  <si>
+    <t>[35769412,34428877]</t>
+  </si>
+  <si>
+    <t>3092505395</t>
   </si>
 </sst>
 </file>
@@ -5874,10 +5919,10 @@
   <dimension ref="A1:AQ313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="Q302" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC63" sqref="AC63"/>
+      <selection pane="bottomRight" activeCell="AF318" sqref="AF318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6314,7 +6359,7 @@
         <v>1796</v>
       </c>
       <c r="S5" t="s">
-        <v>789</v>
+        <v>1818</v>
       </c>
       <c r="AC5" t="s">
         <v>789</v>
@@ -6323,7 +6368,7 @@
         <v>1797</v>
       </c>
       <c r="AE5" t="s">
-        <v>789</v>
+        <v>1819</v>
       </c>
       <c r="AO5" s="9">
         <v>344538810</v>
@@ -6527,7 +6572,7 @@
         <v>805</v>
       </c>
       <c r="S8" t="s">
-        <v>789</v>
+        <v>1823</v>
       </c>
       <c r="AC8" t="s">
         <v>789</v>
@@ -6536,7 +6581,7 @@
         <v>806</v>
       </c>
       <c r="AE8" t="s">
-        <v>789</v>
+        <v>1822</v>
       </c>
       <c r="AO8" s="9">
         <v>627395451</v>
@@ -6737,7 +6782,7 @@
         <v>809</v>
       </c>
       <c r="S11" t="s">
-        <v>789</v>
+        <v>1820</v>
       </c>
       <c r="AC11" t="s">
         <v>810</v>
@@ -6746,7 +6791,7 @@
         <v>811</v>
       </c>
       <c r="AE11" t="s">
-        <v>789</v>
+        <v>1821</v>
       </c>
       <c r="AO11" s="11">
         <v>2358219158</v>
@@ -15422,7 +15467,7 @@
         <v>789</v>
       </c>
       <c r="S137" t="s">
-        <v>789</v>
+        <v>1824</v>
       </c>
       <c r="AC137" t="s">
         <v>1003</v>
@@ -15431,7 +15476,7 @@
         <v>789</v>
       </c>
       <c r="AE137" t="s">
-        <v>789</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="138" spans="1:41" x14ac:dyDescent="0.25">
@@ -26250,7 +26295,60 @@
       </c>
     </row>
     <row r="309" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A309" s="2"/>
+      <c r="A309" s="2">
+        <v>990073</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>1826</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>1826</v>
+      </c>
+      <c r="D309" s="6" t="s">
+        <v>1827</v>
+      </c>
+      <c r="E309" s="6" t="s">
+        <v>1828</v>
+      </c>
+      <c r="G309" t="s">
+        <v>772</v>
+      </c>
+      <c r="H309" t="s">
+        <v>759</v>
+      </c>
+      <c r="I309" t="s">
+        <v>759</v>
+      </c>
+      <c r="J309" t="s">
+        <v>760</v>
+      </c>
+      <c r="K309" t="s">
+        <v>32</v>
+      </c>
+      <c r="L309">
+        <v>201</v>
+      </c>
+      <c r="M309">
+        <v>1</v>
+      </c>
+      <c r="N309">
+        <v>4</v>
+      </c>
+      <c r="O309" t="b">
+        <v>1</v>
+      </c>
+      <c r="P309" t="s">
+        <v>1829</v>
+      </c>
+      <c r="S309" t="s">
+        <v>1830</v>
+      </c>
+      <c r="AE309" t="s">
+        <v>1831</v>
+      </c>
+      <c r="AO309" s="9" t="s">
+        <v>1832</v>
+      </c>
     </row>
     <row r="310" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A310" s="2"/>
@@ -26268,6 +26366,9 @@
   <autoFilter ref="A1:AQ308" xr:uid="{E35BDB71-4614-43CB-874F-BBE88721387F}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="AO309" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
events added to teams sheet
</commit_message>
<xml_diff>
--- a/private/STATIC_DATA_1.xlsx
+++ b/private/STATIC_DATA_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\lolvvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADC61F7-155B-4896-B623-E9DBD7D02F4A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE9FB4B-CE29-40D3-A231-54E91A0303BF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PROS!$A$1:$AR$309</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TEAMS!$A$1:$K$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TEAMS!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5255" uniqueCount="2175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5257" uniqueCount="2175">
   <si>
     <t>nickName</t>
   </si>
@@ -6946,10 +6946,10 @@
   <dimension ref="A1:AR313"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="S29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="AR59" sqref="AR59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27407,7 +27407,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -27431,7 +27431,7 @@
     <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>305</v>
       </c>
@@ -27465,8 +27465,11 @@
       <c r="K1" s="3" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="3" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>101</v>
       </c>
@@ -27501,7 +27504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>102</v>
       </c>
@@ -27536,7 +27539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>103</v>
       </c>
@@ -27571,7 +27574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>104</v>
       </c>
@@ -27606,7 +27609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>105</v>
       </c>
@@ -27641,7 +27644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>106</v>
       </c>
@@ -27676,7 +27679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>107</v>
       </c>
@@ -27711,7 +27714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>108</v>
       </c>
@@ -27746,7 +27749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>109</v>
       </c>
@@ -27781,7 +27784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>110</v>
       </c>
@@ -27816,7 +27819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>111</v>
       </c>
@@ -27842,7 +27845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>112</v>
       </c>
@@ -27868,7 +27871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>113</v>
       </c>
@@ -27894,7 +27897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>114</v>
       </c>
@@ -27920,7 +27923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>201</v>
       </c>
@@ -27953,6 +27956,9 @@
       </c>
       <c r="K16" t="b">
         <v>1</v>
+      </c>
+      <c r="L16" t="s">
+        <v>1834</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -29439,7 +29445,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K63" xr:uid="{EDBF67B8-77AA-43A4-8A86-C9B5D51E87C5}"/>
+  <autoFilter ref="A1:L1" xr:uid="{D4271EDE-385E-4EB2-8A87-9C434923D3B1}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Modification of the team column order
</commit_message>
<xml_diff>
--- a/private/STATIC_DATA_1.xlsx
+++ b/private/STATIC_DATA_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\lolvvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE9FB4B-CE29-40D3-A231-54E91A0303BF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4869F69-08DD-4D50-BB19-AB1FD7D8A449}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6946,10 +6946,10 @@
   <dimension ref="A1:AR313"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="S29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AR59" sqref="AR59"/>
+      <selection pane="bottomRight" activeCell="S39" sqref="B39:S49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27426,8 +27426,8 @@
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -27457,10 +27457,10 @@
         <v>1839</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>1</v>
+        <v>304</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>304</v>
+        <v>1</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>307</v>
@@ -27495,10 +27495,10 @@
         <v>1844</v>
       </c>
       <c r="I2" t="s">
+        <v>760</v>
+      </c>
+      <c r="J2" t="s">
         <v>4</v>
-      </c>
-      <c r="J2" t="s">
-        <v>760</v>
       </c>
       <c r="K2" t="b">
         <v>1</v>
@@ -27530,10 +27530,10 @@
         <v>1851</v>
       </c>
       <c r="I3" t="s">
+        <v>760</v>
+      </c>
+      <c r="J3" t="s">
         <v>4</v>
-      </c>
-      <c r="J3" t="s">
-        <v>760</v>
       </c>
       <c r="K3" t="b">
         <v>1</v>
@@ -27565,10 +27565,10 @@
         <v>1858</v>
       </c>
       <c r="I4" t="s">
+        <v>760</v>
+      </c>
+      <c r="J4" t="s">
         <v>4</v>
-      </c>
-      <c r="J4" t="s">
-        <v>760</v>
       </c>
       <c r="K4" t="b">
         <v>1</v>
@@ -27600,10 +27600,10 @@
         <v>1865</v>
       </c>
       <c r="I5" t="s">
+        <v>760</v>
+      </c>
+      <c r="J5" t="s">
         <v>4</v>
-      </c>
-      <c r="J5" t="s">
-        <v>760</v>
       </c>
       <c r="K5" t="b">
         <v>1</v>
@@ -27635,10 +27635,10 @@
         <v>1872</v>
       </c>
       <c r="I6" t="s">
+        <v>760</v>
+      </c>
+      <c r="J6" t="s">
         <v>4</v>
-      </c>
-      <c r="J6" t="s">
-        <v>760</v>
       </c>
       <c r="K6" t="b">
         <v>1</v>
@@ -27670,10 +27670,10 @@
         <v>1878</v>
       </c>
       <c r="I7" t="s">
+        <v>760</v>
+      </c>
+      <c r="J7" t="s">
         <v>4</v>
-      </c>
-      <c r="J7" t="s">
-        <v>760</v>
       </c>
       <c r="K7" t="b">
         <v>1</v>
@@ -27705,10 +27705,10 @@
         <v>1885</v>
       </c>
       <c r="I8" t="s">
+        <v>760</v>
+      </c>
+      <c r="J8" t="s">
         <v>4</v>
-      </c>
-      <c r="J8" t="s">
-        <v>760</v>
       </c>
       <c r="K8" t="b">
         <v>1</v>
@@ -27740,10 +27740,10 @@
         <v>1892</v>
       </c>
       <c r="I9" t="s">
+        <v>760</v>
+      </c>
+      <c r="J9" t="s">
         <v>4</v>
-      </c>
-      <c r="J9" t="s">
-        <v>760</v>
       </c>
       <c r="K9" t="b">
         <v>1</v>
@@ -27775,10 +27775,10 @@
         <v>1898</v>
       </c>
       <c r="I10" t="s">
+        <v>760</v>
+      </c>
+      <c r="J10" t="s">
         <v>4</v>
-      </c>
-      <c r="J10" t="s">
-        <v>760</v>
       </c>
       <c r="K10" t="b">
         <v>1</v>
@@ -27810,10 +27810,10 @@
         <v>254</v>
       </c>
       <c r="I11" t="s">
+        <v>760</v>
+      </c>
+      <c r="J11" t="s">
         <v>4</v>
-      </c>
-      <c r="J11" t="s">
-        <v>760</v>
       </c>
       <c r="K11" t="b">
         <v>1</v>
@@ -27836,10 +27836,10 @@
         <v>1907</v>
       </c>
       <c r="I12" t="s">
+        <v>760</v>
+      </c>
+      <c r="J12" t="s">
         <v>4</v>
-      </c>
-      <c r="J12" t="s">
-        <v>760</v>
       </c>
       <c r="K12" t="b">
         <v>1</v>
@@ -27862,10 +27862,10 @@
         <v>1912</v>
       </c>
       <c r="I13" t="s">
+        <v>760</v>
+      </c>
+      <c r="J13" t="s">
         <v>4</v>
-      </c>
-      <c r="J13" t="s">
-        <v>760</v>
       </c>
       <c r="K13" t="b">
         <v>1</v>
@@ -27888,10 +27888,10 @@
         <v>1916</v>
       </c>
       <c r="I14" t="s">
+        <v>760</v>
+      </c>
+      <c r="J14" t="s">
         <v>4</v>
-      </c>
-      <c r="J14" t="s">
-        <v>760</v>
       </c>
       <c r="K14" t="b">
         <v>1</v>
@@ -27914,10 +27914,10 @@
         <v>1919</v>
       </c>
       <c r="I15" t="s">
+        <v>760</v>
+      </c>
+      <c r="J15" t="s">
         <v>4</v>
-      </c>
-      <c r="J15" t="s">
-        <v>760</v>
       </c>
       <c r="K15" t="b">
         <v>1</v>
@@ -27949,10 +27949,10 @@
         <v>1924</v>
       </c>
       <c r="I16" t="s">
+        <v>760</v>
+      </c>
+      <c r="J16" t="s">
         <v>32</v>
-      </c>
-      <c r="J16" t="s">
-        <v>760</v>
       </c>
       <c r="K16" t="b">
         <v>1</v>
@@ -27987,10 +27987,10 @@
         <v>1932</v>
       </c>
       <c r="I17" t="s">
+        <v>760</v>
+      </c>
+      <c r="J17" t="s">
         <v>32</v>
-      </c>
-      <c r="J17" t="s">
-        <v>760</v>
       </c>
       <c r="K17" t="b">
         <v>1</v>
@@ -28022,10 +28022,10 @@
         <v>1939</v>
       </c>
       <c r="I18" t="s">
+        <v>760</v>
+      </c>
+      <c r="J18" t="s">
         <v>32</v>
-      </c>
-      <c r="J18" t="s">
-        <v>760</v>
       </c>
       <c r="K18" t="b">
         <v>1</v>
@@ -28057,10 +28057,10 @@
         <v>1945</v>
       </c>
       <c r="I19" t="s">
+        <v>760</v>
+      </c>
+      <c r="J19" t="s">
         <v>32</v>
-      </c>
-      <c r="J19" t="s">
-        <v>760</v>
       </c>
       <c r="K19" t="b">
         <v>1</v>
@@ -28092,10 +28092,10 @@
         <v>1951</v>
       </c>
       <c r="I20" t="s">
+        <v>760</v>
+      </c>
+      <c r="J20" t="s">
         <v>32</v>
-      </c>
-      <c r="J20" t="s">
-        <v>760</v>
       </c>
       <c r="K20" t="b">
         <v>1</v>
@@ -28127,10 +28127,10 @@
         <v>1957</v>
       </c>
       <c r="I21" t="s">
+        <v>760</v>
+      </c>
+      <c r="J21" t="s">
         <v>32</v>
-      </c>
-      <c r="J21" t="s">
-        <v>760</v>
       </c>
       <c r="K21" t="b">
         <v>1</v>
@@ -28162,10 +28162,10 @@
         <v>1964</v>
       </c>
       <c r="I22" t="s">
+        <v>760</v>
+      </c>
+      <c r="J22" t="s">
         <v>32</v>
-      </c>
-      <c r="J22" t="s">
-        <v>760</v>
       </c>
       <c r="K22" t="b">
         <v>1</v>
@@ -28197,10 +28197,10 @@
         <v>1971</v>
       </c>
       <c r="I23" t="s">
+        <v>760</v>
+      </c>
+      <c r="J23" t="s">
         <v>32</v>
-      </c>
-      <c r="J23" t="s">
-        <v>760</v>
       </c>
       <c r="K23" t="b">
         <v>1</v>
@@ -28232,10 +28232,10 @@
         <v>1978</v>
       </c>
       <c r="I24" t="s">
+        <v>760</v>
+      </c>
+      <c r="J24" t="s">
         <v>32</v>
-      </c>
-      <c r="J24" t="s">
-        <v>760</v>
       </c>
       <c r="K24" t="b">
         <v>1</v>
@@ -28267,10 +28267,10 @@
         <v>1984</v>
       </c>
       <c r="I25" t="s">
+        <v>760</v>
+      </c>
+      <c r="J25" t="s">
         <v>32</v>
-      </c>
-      <c r="J25" t="s">
-        <v>760</v>
       </c>
       <c r="K25" t="b">
         <v>1</v>
@@ -28302,10 +28302,10 @@
         <v>1908</v>
       </c>
       <c r="I26" t="s">
+        <v>760</v>
+      </c>
+      <c r="J26" t="s">
         <v>66</v>
-      </c>
-      <c r="J26" t="s">
-        <v>760</v>
       </c>
       <c r="K26" t="b">
         <v>1</v>
@@ -28337,10 +28337,10 @@
         <v>1908</v>
       </c>
       <c r="I27" t="s">
+        <v>760</v>
+      </c>
+      <c r="J27" t="s">
         <v>66</v>
-      </c>
-      <c r="J27" t="s">
-        <v>760</v>
       </c>
       <c r="K27" t="b">
         <v>1</v>
@@ -28372,10 +28372,10 @@
         <v>2001</v>
       </c>
       <c r="I28" t="s">
+        <v>760</v>
+      </c>
+      <c r="J28" t="s">
         <v>66</v>
-      </c>
-      <c r="J28" t="s">
-        <v>760</v>
       </c>
       <c r="K28" t="b">
         <v>1</v>
@@ -28407,10 +28407,10 @@
         <v>2007</v>
       </c>
       <c r="I29" t="s">
+        <v>760</v>
+      </c>
+      <c r="J29" t="s">
         <v>66</v>
-      </c>
-      <c r="J29" t="s">
-        <v>760</v>
       </c>
       <c r="K29" t="b">
         <v>1</v>
@@ -28442,10 +28442,10 @@
         <v>2013</v>
       </c>
       <c r="I30" t="s">
+        <v>760</v>
+      </c>
+      <c r="J30" t="s">
         <v>66</v>
-      </c>
-      <c r="J30" t="s">
-        <v>760</v>
       </c>
       <c r="K30" t="b">
         <v>1</v>
@@ -28477,10 +28477,10 @@
         <v>1908</v>
       </c>
       <c r="I31" t="s">
+        <v>760</v>
+      </c>
+      <c r="J31" t="s">
         <v>66</v>
-      </c>
-      <c r="J31" t="s">
-        <v>760</v>
       </c>
       <c r="K31" t="b">
         <v>1</v>
@@ -28512,10 +28512,10 @@
         <v>1908</v>
       </c>
       <c r="I32" t="s">
+        <v>760</v>
+      </c>
+      <c r="J32" t="s">
         <v>66</v>
-      </c>
-      <c r="J32" t="s">
-        <v>760</v>
       </c>
       <c r="K32" t="b">
         <v>1</v>
@@ -28547,10 +28547,10 @@
         <v>1908</v>
       </c>
       <c r="I33" t="s">
+        <v>760</v>
+      </c>
+      <c r="J33" t="s">
         <v>66</v>
-      </c>
-      <c r="J33" t="s">
-        <v>760</v>
       </c>
       <c r="K33" t="b">
         <v>1</v>
@@ -28573,10 +28573,10 @@
         <v>2031</v>
       </c>
       <c r="I34" t="s">
+        <v>760</v>
+      </c>
+      <c r="J34" t="s">
         <v>66</v>
-      </c>
-      <c r="J34" t="s">
-        <v>760</v>
       </c>
       <c r="K34" t="b">
         <v>1</v>
@@ -28599,10 +28599,10 @@
         <v>2035</v>
       </c>
       <c r="I35" t="s">
+        <v>760</v>
+      </c>
+      <c r="J35" t="s">
         <v>66</v>
-      </c>
-      <c r="J35" t="s">
-        <v>760</v>
       </c>
       <c r="K35" t="b">
         <v>1</v>
@@ -28625,10 +28625,10 @@
         <v>2039</v>
       </c>
       <c r="I36" t="s">
+        <v>760</v>
+      </c>
+      <c r="J36" t="s">
         <v>66</v>
-      </c>
-      <c r="J36" t="s">
-        <v>760</v>
       </c>
       <c r="K36" t="b">
         <v>1</v>
@@ -28660,10 +28660,10 @@
         <v>2045</v>
       </c>
       <c r="I37" t="s">
+        <v>760</v>
+      </c>
+      <c r="J37" t="s">
         <v>66</v>
-      </c>
-      <c r="J37" t="s">
-        <v>760</v>
       </c>
       <c r="K37" t="b">
         <v>1</v>
@@ -28695,10 +28695,10 @@
         <v>2051</v>
       </c>
       <c r="I38" t="s">
+        <v>760</v>
+      </c>
+      <c r="J38" t="s">
         <v>66</v>
-      </c>
-      <c r="J38" t="s">
-        <v>760</v>
       </c>
       <c r="K38" t="b">
         <v>1</v>
@@ -28730,10 +28730,10 @@
         <v>2057</v>
       </c>
       <c r="I39" t="s">
+        <v>760</v>
+      </c>
+      <c r="J39" t="s">
         <v>155</v>
-      </c>
-      <c r="J39" t="s">
-        <v>760</v>
       </c>
       <c r="K39" t="b">
         <v>1</v>
@@ -28765,10 +28765,10 @@
         <v>2063</v>
       </c>
       <c r="I40" t="s">
+        <v>760</v>
+      </c>
+      <c r="J40" t="s">
         <v>155</v>
-      </c>
-      <c r="J40" t="s">
-        <v>760</v>
       </c>
       <c r="K40" t="b">
         <v>1</v>
@@ -28800,10 +28800,10 @@
         <v>2070</v>
       </c>
       <c r="I41" t="s">
+        <v>760</v>
+      </c>
+      <c r="J41" t="s">
         <v>155</v>
-      </c>
-      <c r="J41" t="s">
-        <v>760</v>
       </c>
       <c r="K41" t="b">
         <v>1</v>
@@ -28835,10 +28835,10 @@
         <v>2077</v>
       </c>
       <c r="I42" t="s">
+        <v>760</v>
+      </c>
+      <c r="J42" t="s">
         <v>155</v>
-      </c>
-      <c r="J42" t="s">
-        <v>760</v>
       </c>
       <c r="K42" t="b">
         <v>1</v>
@@ -28861,10 +28861,10 @@
         <v>2081</v>
       </c>
       <c r="I43" t="s">
+        <v>760</v>
+      </c>
+      <c r="J43" t="s">
         <v>155</v>
-      </c>
-      <c r="J43" t="s">
-        <v>760</v>
       </c>
       <c r="K43" t="b">
         <v>1</v>
@@ -28896,10 +28896,10 @@
         <v>2087</v>
       </c>
       <c r="I44" t="s">
+        <v>760</v>
+      </c>
+      <c r="J44" t="s">
         <v>155</v>
-      </c>
-      <c r="J44" t="s">
-        <v>760</v>
       </c>
       <c r="K44" t="b">
         <v>1</v>
@@ -28922,10 +28922,10 @@
         <v>2091</v>
       </c>
       <c r="I45" t="s">
+        <v>760</v>
+      </c>
+      <c r="J45" t="s">
         <v>155</v>
-      </c>
-      <c r="J45" t="s">
-        <v>760</v>
       </c>
       <c r="K45" t="b">
         <v>1</v>
@@ -28948,10 +28948,10 @@
         <v>2095</v>
       </c>
       <c r="I46" t="s">
+        <v>760</v>
+      </c>
+      <c r="J46" t="s">
         <v>155</v>
-      </c>
-      <c r="J46" t="s">
-        <v>760</v>
       </c>
       <c r="K46" t="b">
         <v>1</v>
@@ -28974,10 +28974,10 @@
         <v>2099</v>
       </c>
       <c r="I47" t="s">
+        <v>760</v>
+      </c>
+      <c r="J47" t="s">
         <v>155</v>
-      </c>
-      <c r="J47" t="s">
-        <v>760</v>
       </c>
       <c r="K47" t="b">
         <v>1</v>
@@ -29000,10 +29000,10 @@
         <v>2103</v>
       </c>
       <c r="I48" t="s">
+        <v>760</v>
+      </c>
+      <c r="J48" t="s">
         <v>155</v>
-      </c>
-      <c r="J48" t="s">
-        <v>760</v>
       </c>
       <c r="K48" t="b">
         <v>1</v>
@@ -29026,10 +29026,10 @@
         <v>2107</v>
       </c>
       <c r="I49" t="s">
+        <v>760</v>
+      </c>
+      <c r="J49" t="s">
         <v>155</v>
-      </c>
-      <c r="J49" t="s">
-        <v>760</v>
       </c>
       <c r="K49" t="b">
         <v>1</v>
@@ -29052,10 +29052,10 @@
         <v>2111</v>
       </c>
       <c r="I50" t="s">
+        <v>760</v>
+      </c>
+      <c r="J50" t="s">
         <v>155</v>
-      </c>
-      <c r="J50" t="s">
-        <v>760</v>
       </c>
       <c r="K50" t="b">
         <v>1</v>
@@ -29078,10 +29078,10 @@
         <v>2115</v>
       </c>
       <c r="I51" t="s">
+        <v>760</v>
+      </c>
+      <c r="J51" t="s">
         <v>155</v>
-      </c>
-      <c r="J51" t="s">
-        <v>760</v>
       </c>
       <c r="K51" t="b">
         <v>1</v>
@@ -29104,10 +29104,10 @@
         <v>2119</v>
       </c>
       <c r="I52" t="s">
+        <v>760</v>
+      </c>
+      <c r="J52" t="s">
         <v>155</v>
-      </c>
-      <c r="J52" t="s">
-        <v>760</v>
       </c>
       <c r="K52" t="b">
         <v>1</v>
@@ -29130,10 +29130,10 @@
         <v>2122</v>
       </c>
       <c r="I53" t="s">
+        <v>760</v>
+      </c>
+      <c r="J53" t="s">
         <v>155</v>
-      </c>
-      <c r="J53" t="s">
-        <v>760</v>
       </c>
       <c r="K53" t="b">
         <v>1</v>
@@ -29156,10 +29156,10 @@
         <v>2126</v>
       </c>
       <c r="I54" t="s">
+        <v>760</v>
+      </c>
+      <c r="J54" t="s">
         <v>155</v>
-      </c>
-      <c r="J54" t="s">
-        <v>760</v>
       </c>
       <c r="K54" t="b">
         <v>1</v>
@@ -29191,10 +29191,10 @@
         <v>2132</v>
       </c>
       <c r="I55" t="s">
+        <v>760</v>
+      </c>
+      <c r="J55" t="s">
         <v>211</v>
-      </c>
-      <c r="J55" t="s">
-        <v>760</v>
       </c>
       <c r="K55" t="b">
         <v>1</v>
@@ -29217,10 +29217,10 @@
         <v>2136</v>
       </c>
       <c r="I56" t="s">
+        <v>760</v>
+      </c>
+      <c r="J56" t="s">
         <v>211</v>
-      </c>
-      <c r="J56" t="s">
-        <v>760</v>
       </c>
       <c r="K56" t="b">
         <v>1</v>
@@ -29252,10 +29252,10 @@
         <v>2143</v>
       </c>
       <c r="I57" t="s">
+        <v>760</v>
+      </c>
+      <c r="J57" t="s">
         <v>211</v>
-      </c>
-      <c r="J57" t="s">
-        <v>760</v>
       </c>
       <c r="K57" t="b">
         <v>1</v>
@@ -29287,10 +29287,10 @@
         <v>2149</v>
       </c>
       <c r="I58" t="s">
+        <v>760</v>
+      </c>
+      <c r="J58" t="s">
         <v>211</v>
-      </c>
-      <c r="J58" t="s">
-        <v>760</v>
       </c>
       <c r="K58" t="b">
         <v>1</v>
@@ -29322,10 +29322,10 @@
         <v>2156</v>
       </c>
       <c r="I59" t="s">
+        <v>760</v>
+      </c>
+      <c r="J59" t="s">
         <v>211</v>
-      </c>
-      <c r="J59" t="s">
-        <v>760</v>
       </c>
       <c r="K59" t="b">
         <v>1</v>
@@ -29357,10 +29357,10 @@
         <v>379</v>
       </c>
       <c r="I60" t="s">
+        <v>760</v>
+      </c>
+      <c r="J60" t="s">
         <v>211</v>
-      </c>
-      <c r="J60" t="s">
-        <v>760</v>
       </c>
       <c r="K60" t="b">
         <v>1</v>
@@ -29383,10 +29383,10 @@
         <v>2165</v>
       </c>
       <c r="I61" t="s">
+        <v>760</v>
+      </c>
+      <c r="J61" t="s">
         <v>211</v>
-      </c>
-      <c r="J61" t="s">
-        <v>760</v>
       </c>
       <c r="K61" t="b">
         <v>1</v>
@@ -29409,10 +29409,10 @@
         <v>2169</v>
       </c>
       <c r="I62" t="s">
+        <v>760</v>
+      </c>
+      <c r="J62" t="s">
         <v>211</v>
-      </c>
-      <c r="J62" t="s">
-        <v>760</v>
       </c>
       <c r="K62" t="b">
         <v>1</v>
@@ -29435,10 +29435,10 @@
         <v>2173</v>
       </c>
       <c r="I63" t="s">
+        <v>760</v>
+      </c>
+      <c r="J63" t="s">
         <v>211</v>
-      </c>
-      <c r="J63" t="s">
-        <v>760</v>
       </c>
       <c r="K63" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
missing pro nickNames added
</commit_message>
<xml_diff>
--- a/private/STATIC_DATA_1.xlsx
+++ b/private/STATIC_DATA_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\LolVvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD50D08-ED32-45E0-AB67-8C49DDB75DD8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8710589-8D93-4C93-9D00-A72EB9247BA6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5892" uniqueCount="2475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5897" uniqueCount="2475">
   <si>
     <t>nickName</t>
   </si>
@@ -7876,17 +7876,17 @@
   <dimension ref="A1:AS353"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P321" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE348" sqref="AE348"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
@@ -32069,7 +32069,9 @@
       <c r="B348" s="1" t="s">
         <v>2447</v>
       </c>
-      <c r="C348" s="1"/>
+      <c r="C348" s="1" t="s">
+        <v>2447</v>
+      </c>
       <c r="D348" s="1" t="s">
         <v>2452</v>
       </c>
@@ -32148,7 +32150,9 @@
       <c r="B349" s="1" t="s">
         <v>2448</v>
       </c>
-      <c r="C349" s="1"/>
+      <c r="C349" s="1" t="s">
+        <v>2448</v>
+      </c>
       <c r="D349" s="1" t="s">
         <v>2454</v>
       </c>
@@ -32202,7 +32206,9 @@
       <c r="B350" s="1" t="s">
         <v>2449</v>
       </c>
-      <c r="C350" s="1"/>
+      <c r="C350" s="1" t="s">
+        <v>2449</v>
+      </c>
       <c r="D350" s="1" t="s">
         <v>2456</v>
       </c>
@@ -32256,7 +32262,9 @@
       <c r="B351" s="1" t="s">
         <v>2450</v>
       </c>
-      <c r="C351" s="1"/>
+      <c r="C351" s="1" t="s">
+        <v>2450</v>
+      </c>
       <c r="D351" s="1" t="s">
         <v>2458</v>
       </c>
@@ -32310,7 +32318,9 @@
       <c r="B352" s="1" t="s">
         <v>2451</v>
       </c>
-      <c r="C352" s="1"/>
+      <c r="C352" s="1" t="s">
+        <v>2451</v>
+      </c>
       <c r="D352" s="1" t="s">
         <v>2460</v>
       </c>

</xml_diff>

<commit_message>
MSI pro list update
</commit_message>
<xml_diff>
--- a/private/STATIC_DATA_1.xlsx
+++ b/private/STATIC_DATA_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\LolVvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8710589-8D93-4C93-9D00-A72EB9247BA6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1464BC8-E887-4FF5-B3D3-54CFC5D783FA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5897" uniqueCount="2475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5899" uniqueCount="2477">
   <si>
     <t>nickName</t>
   </si>
@@ -7455,6 +7455,12 @@
   </si>
   <si>
     <t>[107987216]</t>
+  </si>
+  <si>
+    <t>[240064269]</t>
+  </si>
+  <si>
+    <t>[107987200]</t>
   </si>
 </sst>
 </file>
@@ -7876,10 +7882,10 @@
   <dimension ref="A1:AS353"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="P307" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="AE313" sqref="AE313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29184,7 +29190,9 @@
       </c>
       <c r="Q313" s="1"/>
       <c r="R313" s="1"/>
-      <c r="S313" s="1"/>
+      <c r="S313" s="1" t="s">
+        <v>2475</v>
+      </c>
       <c r="T313" s="1"/>
       <c r="U313" s="1"/>
       <c r="V313" s="1"/>
@@ -29196,7 +29204,9 @@
       <c r="AB313" s="1"/>
       <c r="AC313" s="1"/>
       <c r="AD313" s="1"/>
-      <c r="AE313" s="1"/>
+      <c r="AE313" s="1" t="s">
+        <v>2476</v>
+      </c>
       <c r="AF313" s="1"/>
       <c r="AG313" s="1"/>
       <c r="AH313" s="1"/>

</xml_diff>

<commit_message>
MSI pro list update, EVOS added ...
</commit_message>
<xml_diff>
--- a/private/STATIC_DATA_1.xlsx
+++ b/private/STATIC_DATA_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\LolVvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E5B330-1F9E-434F-A3BD-DD763B7AC5BD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0388E4-5A81-40CF-9328-F78EDB6E65FF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5899" uniqueCount="2481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6133" uniqueCount="2547">
   <si>
     <t>nickName</t>
   </si>
@@ -7473,13 +7473,211 @@
   </si>
   <si>
     <t>sEiya</t>
+  </si>
+  <si>
+    <t>Hanabi</t>
+  </si>
+  <si>
+    <t>Moojin</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>Stark</t>
+  </si>
+  <si>
+    <t>YiJin</t>
+  </si>
+  <si>
+    <t>Warzone</t>
+  </si>
+  <si>
+    <t>Slay</t>
+  </si>
+  <si>
+    <t>RonOP</t>
+  </si>
+  <si>
+    <t>Công Minh</t>
+  </si>
+  <si>
+    <t>Nguyễn</t>
+  </si>
+  <si>
+    <t>Lê Hải Đăng</t>
+  </si>
+  <si>
+    <t>Đoàn</t>
+  </si>
+  <si>
+    <t>Văn Ngọc Sơn</t>
+  </si>
+  <si>
+    <t>Ngọc Hùng</t>
+  </si>
+  <si>
+    <t>Lê</t>
+  </si>
+  <si>
+    <t>Thiên Hàn</t>
+  </si>
+  <si>
+    <t>VN</t>
+  </si>
+  <si>
+    <t>vn</t>
+  </si>
+  <si>
+    <t>Chia-Hsiang</t>
+  </si>
+  <si>
+    <t>TW</t>
+  </si>
+  <si>
+    <t>Moo-jin</t>
+  </si>
+  <si>
+    <t>Kuan-Ting</t>
+  </si>
+  <si>
+    <t>hanabi_2018.png</t>
+  </si>
+  <si>
+    <t>stark_2018.png</t>
+  </si>
+  <si>
+    <t>moojin_2018.png</t>
+  </si>
+  <si>
+    <t>morning_2018.png</t>
+  </si>
+  <si>
+    <t>yijin_2018.png</t>
+  </si>
+  <si>
+    <t>warzone_2018.png</t>
+  </si>
+  <si>
+    <t>slay_2018.png</t>
+  </si>
+  <si>
+    <t>ronop_2018.png</t>
+  </si>
+  <si>
+    <t>evosesports</t>
+  </si>
+  <si>
+    <t>EVOS Esports</t>
+  </si>
+  <si>
+    <t>EVS</t>
+  </si>
+  <si>
+    <t>logo_evosesports_2018.png</t>
+  </si>
+  <si>
+    <t>Ngô</t>
+  </si>
+  <si>
+    <t>Mạnh Quyền</t>
+  </si>
+  <si>
+    <t>Violet</t>
+  </si>
+  <si>
+    <t>[240064265]</t>
+  </si>
+  <si>
+    <t>[107957164]</t>
+  </si>
+  <si>
+    <t>[107957163]</t>
+  </si>
+  <si>
+    <t>[240064263]</t>
+  </si>
+  <si>
+    <t>[240064802]</t>
+  </si>
+  <si>
+    <t>[107957162]</t>
+  </si>
+  <si>
+    <t>[240064803]</t>
+  </si>
+  <si>
+    <t>[107987193]</t>
+  </si>
+  <si>
+    <t>[240064358]</t>
+  </si>
+  <si>
+    <t>[107977106]</t>
+  </si>
+  <si>
+    <t>[240064620]</t>
+  </si>
+  <si>
+    <t>[107957183]</t>
+  </si>
+  <si>
+    <t>[240064621]</t>
+  </si>
+  <si>
+    <t>[107977130]</t>
+  </si>
+  <si>
+    <t>[240065119]</t>
+  </si>
+  <si>
+    <t>[107977131]</t>
+  </si>
+  <si>
+    <t>[240064380]</t>
+  </si>
+  <si>
+    <t>[107987221]</t>
+  </si>
+  <si>
+    <t>[240064381]</t>
+  </si>
+  <si>
+    <t>[107987222]</t>
+  </si>
+  <si>
+    <t>[230583110]</t>
+  </si>
+  <si>
+    <t>[94007523]</t>
+  </si>
+  <si>
+    <t>[240064549]</t>
+  </si>
+  <si>
+    <t>[240064707]</t>
+  </si>
+  <si>
+    <t>[107987191]</t>
+  </si>
+  <si>
+    <t>[240064192]</t>
+  </si>
+  <si>
+    <t>[107977105]</t>
+  </si>
+  <si>
+    <t>[240064095]</t>
+  </si>
+  <si>
+    <t>[107957158]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7508,6 +7706,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -7551,7 +7755,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -7577,6 +7781,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -7891,13 +8096,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS353"/>
+  <dimension ref="A1:AS361"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C302" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="R95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C312" sqref="C312"/>
+      <selection pane="bottomRight" activeCell="AR108" sqref="AR108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15366,7 +15571,7 @@
         <v>789</v>
       </c>
       <c r="S106" t="s">
-        <v>789</v>
+        <v>2543</v>
       </c>
       <c r="AC106" t="s">
         <v>980</v>
@@ -15375,7 +15580,7 @@
         <v>789</v>
       </c>
       <c r="AE106" t="s">
-        <v>789</v>
+        <v>2544</v>
       </c>
       <c r="AR106" t="s">
         <v>1829</v>
@@ -15434,7 +15639,7 @@
         <v>789</v>
       </c>
       <c r="S107" t="s">
-        <v>789</v>
+        <v>2541</v>
       </c>
       <c r="AC107" t="s">
         <v>1623</v>
@@ -15443,7 +15648,7 @@
         <v>789</v>
       </c>
       <c r="AE107" t="s">
-        <v>789</v>
+        <v>2542</v>
       </c>
       <c r="AR107" t="s">
         <v>1829</v>
@@ -15505,7 +15710,7 @@
         <v>789</v>
       </c>
       <c r="S108" t="s">
-        <v>789</v>
+        <v>2540</v>
       </c>
       <c r="AC108" t="s">
         <v>1806</v>
@@ -15514,7 +15719,7 @@
         <v>789</v>
       </c>
       <c r="AE108" t="s">
-        <v>789</v>
+        <v>2540</v>
       </c>
       <c r="AO108" s="10" t="s">
         <v>1776</v>
@@ -16490,16 +16695,13 @@
         <v>789</v>
       </c>
       <c r="S122" t="s">
-        <v>789</v>
+        <v>2545</v>
       </c>
       <c r="AC122" t="s">
         <v>1756</v>
       </c>
-      <c r="AD122" t="s">
-        <v>789</v>
-      </c>
       <c r="AE122" t="s">
-        <v>789</v>
+        <v>2546</v>
       </c>
       <c r="AO122" s="9">
         <v>4742883794</v>
@@ -23177,7 +23379,7 @@
         <v>789</v>
       </c>
       <c r="S224" t="s">
-        <v>789</v>
+        <v>2534</v>
       </c>
       <c r="AC224" t="s">
         <v>1077</v>
@@ -23186,7 +23388,7 @@
         <v>789</v>
       </c>
       <c r="AE224" t="s">
-        <v>789</v>
+        <v>2535</v>
       </c>
       <c r="AR224" t="s">
         <v>1829</v>
@@ -23245,7 +23447,7 @@
         <v>789</v>
       </c>
       <c r="S225" t="s">
-        <v>789</v>
+        <v>2532</v>
       </c>
       <c r="AC225" t="s">
         <v>1078</v>
@@ -23254,7 +23456,7 @@
         <v>789</v>
       </c>
       <c r="AE225" t="s">
-        <v>789</v>
+        <v>2533</v>
       </c>
       <c r="AR225" t="s">
         <v>1829</v>
@@ -23316,7 +23518,7 @@
         <v>789</v>
       </c>
       <c r="S226" t="s">
-        <v>789</v>
+        <v>2536</v>
       </c>
       <c r="AC226" t="s">
         <v>1079</v>
@@ -23325,7 +23527,7 @@
         <v>789</v>
       </c>
       <c r="AE226" t="s">
-        <v>789</v>
+        <v>2537</v>
       </c>
       <c r="AR226" t="s">
         <v>1829</v>
@@ -29710,7 +29912,9 @@
       </c>
       <c r="Q319" s="1"/>
       <c r="R319" s="1"/>
-      <c r="S319" s="1"/>
+      <c r="S319" s="1" t="s">
+        <v>2538</v>
+      </c>
       <c r="T319" s="1"/>
       <c r="U319" s="1"/>
       <c r="V319" s="1"/>
@@ -29722,7 +29926,9 @@
       <c r="AB319" s="1"/>
       <c r="AC319" s="1"/>
       <c r="AD319" s="1"/>
-      <c r="AE319" s="1"/>
+      <c r="AE319" s="1" t="s">
+        <v>2539</v>
+      </c>
       <c r="AF319" s="1"/>
       <c r="AG319" s="1"/>
       <c r="AH319" s="1"/>
@@ -32162,7 +32368,9 @@
       <c r="AO348" s="14"/>
       <c r="AP348" s="1"/>
       <c r="AQ348" s="1"/>
-      <c r="AR348" s="1"/>
+      <c r="AR348" s="1" t="s">
+        <v>1829</v>
+      </c>
       <c r="AS348" s="1"/>
     </row>
     <row r="349" spans="1:45" x14ac:dyDescent="0.25">
@@ -32220,6 +32428,9 @@
       <c r="AE349" s="1" t="s">
         <v>2469</v>
       </c>
+      <c r="AR349" s="1" t="s">
+        <v>1829</v>
+      </c>
     </row>
     <row r="350" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A350" s="2">
@@ -32276,6 +32487,9 @@
       <c r="AE350" s="1" t="s">
         <v>2471</v>
       </c>
+      <c r="AR350" s="1" t="s">
+        <v>1829</v>
+      </c>
     </row>
     <row r="351" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A351" s="2">
@@ -32332,6 +32546,9 @@
       <c r="AE351" t="s">
         <v>2467</v>
       </c>
+      <c r="AR351" s="1" t="s">
+        <v>1829</v>
+      </c>
     </row>
     <row r="352" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A352" s="2">
@@ -32386,15 +32603,473 @@
       <c r="AE352" t="s">
         <v>2465</v>
       </c>
-    </row>
-    <row r="353" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B353" s="1"/>
-      <c r="C353" s="1"/>
-      <c r="D353" s="1"/>
-      <c r="E353" s="1"/>
+      <c r="AR352" s="1" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="353" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A353" s="2">
+        <v>990117</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>2481</v>
+      </c>
+      <c r="C353" s="1" t="s">
+        <v>2481</v>
+      </c>
+      <c r="D353" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="E353" s="6" t="s">
+        <v>2499</v>
+      </c>
       <c r="F353" s="13"/>
-      <c r="G353" s="1"/>
-      <c r="H353" s="1"/>
+      <c r="G353" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="H353" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="I353" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="J353" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K353" s="1" t="s">
+        <v>2500</v>
+      </c>
+      <c r="L353">
+        <v>504</v>
+      </c>
+      <c r="M353">
+        <v>1</v>
+      </c>
+      <c r="N353" s="1">
+        <v>3</v>
+      </c>
+      <c r="O353" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P353" t="s">
+        <v>2503</v>
+      </c>
+      <c r="S353" t="s">
+        <v>2528</v>
+      </c>
+      <c r="AE353" t="s">
+        <v>2529</v>
+      </c>
+      <c r="AR353" s="1" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="354" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A354" s="2">
+        <v>990118</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>2482</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>2482</v>
+      </c>
+      <c r="D354" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E354" s="6" t="s">
+        <v>2501</v>
+      </c>
+      <c r="G354" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="H354" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="I354" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="J354" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K354" s="1" t="s">
+        <v>2500</v>
+      </c>
+      <c r="L354">
+        <v>504</v>
+      </c>
+      <c r="M354">
+        <v>2</v>
+      </c>
+      <c r="N354" s="1">
+        <v>3</v>
+      </c>
+      <c r="O354" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P354" t="s">
+        <v>2505</v>
+      </c>
+      <c r="S354" t="s">
+        <v>2530</v>
+      </c>
+      <c r="AE354" t="s">
+        <v>2531</v>
+      </c>
+      <c r="AR354" s="1" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="355" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A355" s="2">
+        <v>990119</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>2483</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>2483</v>
+      </c>
+      <c r="D355" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E355" s="6" t="s">
+        <v>2502</v>
+      </c>
+      <c r="F355" s="5">
+        <v>34995</v>
+      </c>
+      <c r="G355" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="H355" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="I355" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="J355" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K355" s="1" t="s">
+        <v>2500</v>
+      </c>
+      <c r="L355">
+        <v>504</v>
+      </c>
+      <c r="M355">
+        <v>2</v>
+      </c>
+      <c r="N355" s="1">
+        <v>3</v>
+      </c>
+      <c r="O355" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P355" t="s">
+        <v>2506</v>
+      </c>
+      <c r="AR355" s="1" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="356" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A356" s="2">
+        <v>990120</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>2484</v>
+      </c>
+      <c r="C356" s="1" t="s">
+        <v>2484</v>
+      </c>
+      <c r="D356" t="s">
+        <v>531</v>
+      </c>
+      <c r="E356" s="17" t="s">
+        <v>2489</v>
+      </c>
+      <c r="F356" s="5">
+        <v>35789</v>
+      </c>
+      <c r="G356" t="s">
+        <v>2498</v>
+      </c>
+      <c r="H356" t="s">
+        <v>759</v>
+      </c>
+      <c r="I356" t="s">
+        <v>759</v>
+      </c>
+      <c r="J356" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K356" s="1" t="s">
+        <v>2497</v>
+      </c>
+      <c r="L356">
+        <v>909</v>
+      </c>
+      <c r="M356">
+        <v>1</v>
+      </c>
+      <c r="N356">
+        <v>3</v>
+      </c>
+      <c r="O356" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P356" t="s">
+        <v>2504</v>
+      </c>
+      <c r="S356" t="s">
+        <v>2522</v>
+      </c>
+      <c r="AE356" t="s">
+        <v>2523</v>
+      </c>
+      <c r="AR356" s="1" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="357" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A357" s="2">
+        <v>990121</v>
+      </c>
+      <c r="B357" s="1" t="s">
+        <v>2485</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>2485</v>
+      </c>
+      <c r="D357" t="s">
+        <v>2490</v>
+      </c>
+      <c r="E357" t="s">
+        <v>2491</v>
+      </c>
+      <c r="F357" s="5">
+        <v>36797</v>
+      </c>
+      <c r="G357" t="s">
+        <v>2498</v>
+      </c>
+      <c r="H357" t="s">
+        <v>762</v>
+      </c>
+      <c r="I357" t="s">
+        <v>762</v>
+      </c>
+      <c r="J357" t="s">
+        <v>760</v>
+      </c>
+      <c r="K357" s="1" t="s">
+        <v>2497</v>
+      </c>
+      <c r="L357">
+        <v>909</v>
+      </c>
+      <c r="M357">
+        <v>2</v>
+      </c>
+      <c r="N357">
+        <v>3</v>
+      </c>
+      <c r="O357" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P357" t="s">
+        <v>2507</v>
+      </c>
+      <c r="S357" t="s">
+        <v>2526</v>
+      </c>
+      <c r="AE357" t="s">
+        <v>2527</v>
+      </c>
+      <c r="AR357" s="1" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="358" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A358" s="2">
+        <v>990122</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>2486</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>2486</v>
+      </c>
+      <c r="D358" t="s">
+        <v>2492</v>
+      </c>
+      <c r="E358" t="s">
+        <v>2493</v>
+      </c>
+      <c r="F358" s="5">
+        <v>34661</v>
+      </c>
+      <c r="G358" t="s">
+        <v>2498</v>
+      </c>
+      <c r="H358" t="s">
+        <v>763</v>
+      </c>
+      <c r="I358" t="s">
+        <v>763</v>
+      </c>
+      <c r="J358" t="s">
+        <v>760</v>
+      </c>
+      <c r="K358" s="1" t="s">
+        <v>2497</v>
+      </c>
+      <c r="L358">
+        <v>909</v>
+      </c>
+      <c r="M358">
+        <v>3</v>
+      </c>
+      <c r="N358">
+        <v>3</v>
+      </c>
+      <c r="O358" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="P358" t="s">
+        <v>2508</v>
+      </c>
+      <c r="S358" t="s">
+        <v>2524</v>
+      </c>
+      <c r="AE358" t="s">
+        <v>2525</v>
+      </c>
+      <c r="AR358" s="1" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="359" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A359" s="2">
+        <v>990123</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>2487</v>
+      </c>
+      <c r="C359" s="1" t="s">
+        <v>2487</v>
+      </c>
+      <c r="D359" t="s">
+        <v>2490</v>
+      </c>
+      <c r="E359" t="s">
+        <v>2494</v>
+      </c>
+      <c r="F359" s="5">
+        <v>35639</v>
+      </c>
+      <c r="G359" t="s">
+        <v>2498</v>
+      </c>
+      <c r="H359" t="s">
+        <v>764</v>
+      </c>
+      <c r="I359" t="s">
+        <v>765</v>
+      </c>
+      <c r="J359" t="s">
+        <v>760</v>
+      </c>
+      <c r="K359" s="1" t="s">
+        <v>2497</v>
+      </c>
+      <c r="L359">
+        <v>909</v>
+      </c>
+      <c r="M359">
+        <v>4</v>
+      </c>
+      <c r="N359">
+        <v>3</v>
+      </c>
+      <c r="O359" t="b">
+        <v>1</v>
+      </c>
+      <c r="P359" t="s">
+        <v>2509</v>
+      </c>
+      <c r="S359" t="s">
+        <v>2521</v>
+      </c>
+      <c r="AE359" t="s">
+        <v>2520</v>
+      </c>
+      <c r="AR359" s="1" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="360" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A360" s="2">
+        <v>990124</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>2488</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>2488</v>
+      </c>
+      <c r="D360" s="17" t="s">
+        <v>2495</v>
+      </c>
+      <c r="E360" t="s">
+        <v>2496</v>
+      </c>
+      <c r="F360" s="5">
+        <v>36102</v>
+      </c>
+      <c r="G360" t="s">
+        <v>2498</v>
+      </c>
+      <c r="H360" t="s">
+        <v>764</v>
+      </c>
+      <c r="I360" t="s">
+        <v>767</v>
+      </c>
+      <c r="J360" t="s">
+        <v>760</v>
+      </c>
+      <c r="K360" s="1" t="s">
+        <v>2497</v>
+      </c>
+      <c r="L360">
+        <v>909</v>
+      </c>
+      <c r="M360">
+        <v>5</v>
+      </c>
+      <c r="N360" s="1">
+        <v>3</v>
+      </c>
+      <c r="O360" t="b">
+        <v>1</v>
+      </c>
+      <c r="P360" t="s">
+        <v>2510</v>
+      </c>
+      <c r="S360" t="s">
+        <v>2518</v>
+      </c>
+      <c r="AE360" t="s">
+        <v>2519</v>
+      </c>
+      <c r="AR360" s="1" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="361" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AR361" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AR309" xr:uid="{BA6111F9-BD81-4878-B56C-AE66D059C8C0}"/>
@@ -32411,10 +33086,10 @@
   <dimension ref="A1:N72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C55" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B67" sqref="B67"/>
+      <selection pane="bottomRight" activeCell="L77" sqref="L77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34763,17 +35438,42 @@
       <c r="N71" s="1"/>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
+      <c r="A72" s="2">
+        <v>909</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>2511</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>2512</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>2513</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>2514</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>2515</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>2516</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>2517</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>2497</v>
+      </c>
+      <c r="K72" t="b">
+        <v>1</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>1829</v>
+      </c>
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
     </row>

</xml_diff>

<commit_message>
SKT Thal account and summoner id fixed
</commit_message>
<xml_diff>
--- a/private/STATIC_DATA_1.xlsx
+++ b/private/STATIC_DATA_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\lolvvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0ECA4A62-F9DA-43B3-A3F0-C7B4E6D2B010}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AA6E8EBB-9088-4CEA-BE24-B241A1DFD443}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7682,12 +7682,6 @@
     <t>thal_2018.png</t>
   </si>
   <si>
-    <t>[4355672]</t>
-  </si>
-  <si>
-    <t>[5570714]</t>
-  </si>
-  <si>
     <t>Blossom</t>
   </si>
   <si>
@@ -7740,6 +7734,12 @@
   </si>
   <si>
     <t>[65821228,17596207]</t>
+  </si>
+  <si>
+    <t>[201236882]</t>
+  </si>
+  <si>
+    <t>[16810685]</t>
   </si>
 </sst>
 </file>
@@ -8168,10 +8168,10 @@
   <dimension ref="A1:AS365"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H320" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M352" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F358" sqref="F358"/>
+      <selection pane="bottomRight" activeCell="AC362" sqref="AC362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33184,10 +33184,10 @@
         <v>2549</v>
       </c>
       <c r="Q361" t="s">
-        <v>2550</v>
+        <v>2568</v>
       </c>
       <c r="AC361" t="s">
-        <v>2551</v>
+        <v>2569</v>
       </c>
       <c r="AR361" s="1"/>
     </row>
@@ -33196,16 +33196,16 @@
         <v>990126</v>
       </c>
       <c r="B362" t="s">
-        <v>2552</v>
+        <v>2550</v>
       </c>
       <c r="C362" t="s">
-        <v>2552</v>
+        <v>2550</v>
       </c>
       <c r="D362" s="17" t="s">
         <v>423</v>
       </c>
       <c r="E362" t="s">
-        <v>2553</v>
+        <v>2551</v>
       </c>
       <c r="G362" t="s">
         <v>768</v>
@@ -33235,13 +33235,13 @@
         <v>1</v>
       </c>
       <c r="P362" t="s">
+        <v>2552</v>
+      </c>
+      <c r="Q362" t="s">
+        <v>2553</v>
+      </c>
+      <c r="AC362" t="s">
         <v>2554</v>
-      </c>
-      <c r="Q362" t="s">
-        <v>2555</v>
-      </c>
-      <c r="AC362" t="s">
-        <v>2556</v>
       </c>
     </row>
     <row r="363" spans="1:44" x14ac:dyDescent="0.25">
@@ -33249,10 +33249,10 @@
         <v>990127</v>
       </c>
       <c r="B363" t="s">
-        <v>2557</v>
+        <v>2555</v>
       </c>
       <c r="C363" t="s">
-        <v>2557</v>
+        <v>2555</v>
       </c>
       <c r="D363" t="s">
         <v>344</v>
@@ -33291,13 +33291,13 @@
         <v>1</v>
       </c>
       <c r="P363" t="s">
+        <v>2556</v>
+      </c>
+      <c r="Q363" t="s">
+        <v>2557</v>
+      </c>
+      <c r="AC363" t="s">
         <v>2558</v>
-      </c>
-      <c r="Q363" t="s">
-        <v>2559</v>
-      </c>
-      <c r="AC363" t="s">
-        <v>2560</v>
       </c>
     </row>
     <row r="364" spans="1:44" x14ac:dyDescent="0.25">
@@ -33305,16 +33305,16 @@
         <v>990128</v>
       </c>
       <c r="B364" t="s">
-        <v>2561</v>
+        <v>2559</v>
       </c>
       <c r="C364" t="s">
-        <v>2561</v>
+        <v>2559</v>
       </c>
       <c r="D364" t="s">
         <v>426</v>
       </c>
       <c r="E364" t="s">
-        <v>2562</v>
+        <v>2560</v>
       </c>
       <c r="G364" t="s">
         <v>768</v>
@@ -33347,10 +33347,10 @@
         <v>1260</v>
       </c>
       <c r="Q364" t="s">
-        <v>2563</v>
+        <v>2561</v>
       </c>
       <c r="AC364" t="s">
-        <v>2564</v>
+        <v>2562</v>
       </c>
     </row>
     <row r="365" spans="1:44" x14ac:dyDescent="0.25">
@@ -33358,16 +33358,16 @@
         <v>990129</v>
       </c>
       <c r="B365" t="s">
-        <v>2565</v>
+        <v>2563</v>
       </c>
       <c r="C365" t="s">
-        <v>2565</v>
+        <v>2563</v>
       </c>
       <c r="D365" t="s">
         <v>338</v>
       </c>
       <c r="E365" t="s">
-        <v>2566</v>
+        <v>2564</v>
       </c>
       <c r="G365" t="s">
         <v>768</v>
@@ -33397,13 +33397,13 @@
         <v>1</v>
       </c>
       <c r="P365" t="s">
+        <v>2565</v>
+      </c>
+      <c r="Q365" t="s">
+        <v>2566</v>
+      </c>
+      <c r="AC365" t="s">
         <v>2567</v>
-      </c>
-      <c r="Q365" t="s">
-        <v>2568</v>
-      </c>
-      <c r="AC365" t="s">
-        <v>2569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sneaky and Zayzal Bootcamp accounts
</commit_message>
<xml_diff>
--- a/private/STATIC_DATA_1.xlsx
+++ b/private/STATIC_DATA_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\LolVvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F105C9-B150-4057-AACB-E1B3CB996CE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0018E1EB-39AB-44FC-8E22-70E78E106A82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6647" uniqueCount="2801">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6607" uniqueCount="2805">
   <si>
     <t>nickName</t>
   </si>
@@ -8433,6 +8433,18 @@
   </si>
   <si>
     <t>[76360143]</t>
+  </si>
+  <si>
+    <t>[2034933795614528]</t>
+  </si>
+  <si>
+    <t>[76820876]</t>
+  </si>
+  <si>
+    <t>[2034933802840032]</t>
+  </si>
+  <si>
+    <t>[76640825]</t>
   </si>
 </sst>
 </file>
@@ -8863,10 +8875,10 @@
   <dimension ref="A1:AS413"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Y56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="N362" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC57" sqref="AC57"/>
+      <selection pane="bottomRight" activeCell="O368" sqref="O368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10375,7 +10387,7 @@
         <v>2505</v>
       </c>
       <c r="Q20" t="s">
-        <v>788</v>
+        <v>2801</v>
       </c>
       <c r="R20" t="s">
         <v>827</v>
@@ -10384,7 +10396,7 @@
         <v>788</v>
       </c>
       <c r="AC20" t="s">
-        <v>788</v>
+        <v>2802</v>
       </c>
       <c r="AD20" t="s">
         <v>828</v>
@@ -34250,10 +34262,16 @@
         <v>3</v>
       </c>
       <c r="O368" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P368" t="s">
         <v>2639</v>
+      </c>
+      <c r="Q368" t="s">
+        <v>2803</v>
+      </c>
+      <c r="AC368" t="s">
+        <v>2804</v>
       </c>
     </row>
     <row r="369" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
NA  LCS pro update
</commit_message>
<xml_diff>
--- a/private/STATIC_DATA_1.xlsx
+++ b/private/STATIC_DATA_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\LolVvv\Assets\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32510AB-3B31-4C8F-A733-5941EEA1CD88}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FD3527-4497-485A-93F2-03C692A06A9E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6703" uniqueCount="2860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6666" uniqueCount="2860">
   <si>
     <t>nickName</t>
   </si>
@@ -9044,10 +9044,10 @@
   <dimension ref="A1:AS421"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K274" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K261" sqref="K261:K311"/>
+      <selection pane="bottomRight" activeCell="L110" sqref="L110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10940,8 +10940,8 @@
       <c r="K26" t="s">
         <v>4</v>
       </c>
-      <c r="L26">
-        <v>101</v>
+      <c r="L26" s="1">
+        <v>111</v>
       </c>
       <c r="M26">
         <v>1</v>
@@ -11011,7 +11011,7 @@
       <c r="K27" t="s">
         <v>4</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="1">
         <v>101</v>
       </c>
       <c r="M27">
@@ -11076,12 +11076,6 @@
       <c r="J28" t="s">
         <v>758</v>
       </c>
-      <c r="K28" t="s">
-        <v>4</v>
-      </c>
-      <c r="L28">
-        <v>101</v>
-      </c>
       <c r="M28">
         <v>1</v>
       </c>
@@ -11213,7 +11207,7 @@
         <v>4</v>
       </c>
       <c r="L30">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="M30">
         <v>2</v>
@@ -11407,12 +11401,6 @@
       <c r="J33" t="s">
         <v>758</v>
       </c>
-      <c r="K33" t="s">
-        <v>4</v>
-      </c>
-      <c r="L33">
-        <v>101</v>
-      </c>
       <c r="M33">
         <v>4</v>
       </c>
@@ -11466,12 +11454,6 @@
       <c r="J34" t="s">
         <v>758</v>
       </c>
-      <c r="K34" t="s">
-        <v>4</v>
-      </c>
-      <c r="L34">
-        <v>101</v>
-      </c>
       <c r="M34">
         <v>1</v>
       </c>
@@ -11513,12 +11495,6 @@
       <c r="J35" t="s">
         <v>758</v>
       </c>
-      <c r="K35" t="s">
-        <v>4</v>
-      </c>
-      <c r="L35">
-        <v>101</v>
-      </c>
       <c r="M35">
         <v>5</v>
       </c>
@@ -11708,12 +11684,6 @@
       <c r="J38" t="s">
         <v>758</v>
       </c>
-      <c r="K38" t="s">
-        <v>4</v>
-      </c>
-      <c r="L38">
-        <v>103</v>
-      </c>
       <c r="M38">
         <v>2</v>
       </c>
@@ -11780,7 +11750,7 @@
         <v>4</v>
       </c>
       <c r="L39">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="M39">
         <v>3</v>
@@ -11918,12 +11888,8 @@
       <c r="J41" s="1" t="s">
         <v>758</v>
       </c>
-      <c r="K41" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L41" s="1">
-        <v>103</v>
-      </c>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
       <c r="M41" s="1">
         <v>2</v>
       </c>
@@ -12002,12 +11968,6 @@
       <c r="J42" t="s">
         <v>758</v>
       </c>
-      <c r="K42" t="s">
-        <v>4</v>
-      </c>
-      <c r="L42">
-        <v>103</v>
-      </c>
       <c r="M42">
         <v>4</v>
       </c>
@@ -12108,12 +12068,6 @@
       <c r="J44" t="s">
         <v>758</v>
       </c>
-      <c r="K44" t="s">
-        <v>4</v>
-      </c>
-      <c r="L44">
-        <v>103</v>
-      </c>
       <c r="M44">
         <v>5</v>
       </c>
@@ -12342,7 +12296,7 @@
         <v>4</v>
       </c>
       <c r="L48">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="M48">
         <v>3</v>
@@ -12484,7 +12438,7 @@
         <v>4</v>
       </c>
       <c r="L50">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="M50">
         <v>5</v>
@@ -12854,12 +12808,6 @@
       <c r="J56" t="s">
         <v>758</v>
       </c>
-      <c r="K56" t="s">
-        <v>4</v>
-      </c>
-      <c r="L56">
-        <v>104</v>
-      </c>
       <c r="M56">
         <v>1</v>
       </c>
@@ -12904,12 +12852,6 @@
       <c r="J57" t="s">
         <v>758</v>
       </c>
-      <c r="K57" t="s">
-        <v>4</v>
-      </c>
-      <c r="L57">
-        <v>107</v>
-      </c>
       <c r="M57">
         <v>1</v>
       </c>
@@ -12972,12 +12914,6 @@
       <c r="J58" t="s">
         <v>758</v>
       </c>
-      <c r="K58" t="s">
-        <v>4</v>
-      </c>
-      <c r="L58">
-        <v>107</v>
-      </c>
       <c r="M58">
         <v>2</v>
       </c>
@@ -13040,12 +12976,6 @@
       <c r="J59" t="s">
         <v>758</v>
       </c>
-      <c r="K59" t="s">
-        <v>4</v>
-      </c>
-      <c r="L59">
-        <v>107</v>
-      </c>
       <c r="M59">
         <v>3</v>
       </c>
@@ -13186,7 +13116,7 @@
         <v>4</v>
       </c>
       <c r="L61" s="1">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="M61" s="1">
         <v>2</v>
@@ -13270,7 +13200,7 @@
         <v>4</v>
       </c>
       <c r="L62" s="1">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="M62" s="1">
         <v>5</v>
@@ -13350,12 +13280,8 @@
       <c r="J63" s="1" t="s">
         <v>758</v>
       </c>
-      <c r="K63" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L63" s="1">
-        <v>107</v>
-      </c>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
       <c r="M63" s="1"/>
       <c r="N63" s="1">
         <v>3</v>
@@ -13429,12 +13355,6 @@
       <c r="J64" t="s">
         <v>758</v>
       </c>
-      <c r="K64" t="s">
-        <v>4</v>
-      </c>
-      <c r="L64">
-        <v>107</v>
-      </c>
       <c r="M64">
         <v>4</v>
       </c>
@@ -13476,12 +13396,6 @@
       <c r="J65" t="s">
         <v>758</v>
       </c>
-      <c r="K65" t="s">
-        <v>4</v>
-      </c>
-      <c r="L65">
-        <v>107</v>
-      </c>
       <c r="M65">
         <v>5</v>
       </c>
@@ -13523,12 +13437,6 @@
       <c r="J66" t="s">
         <v>758</v>
       </c>
-      <c r="K66" t="s">
-        <v>4</v>
-      </c>
-      <c r="L66">
-        <v>107</v>
-      </c>
       <c r="M66">
         <v>5</v>
       </c>
@@ -13579,12 +13487,6 @@
       <c r="J67" t="s">
         <v>758</v>
       </c>
-      <c r="K67" t="s">
-        <v>4</v>
-      </c>
-      <c r="L67">
-        <v>107</v>
-      </c>
       <c r="M67">
         <v>1</v>
       </c>
@@ -13626,12 +13528,6 @@
       <c r="J68" t="s">
         <v>758</v>
       </c>
-      <c r="K68" t="s">
-        <v>4</v>
-      </c>
-      <c r="L68">
-        <v>107</v>
-      </c>
       <c r="M68">
         <v>3</v>
       </c>
@@ -13682,12 +13578,6 @@
       <c r="J69" t="s">
         <v>758</v>
       </c>
-      <c r="K69" t="s">
-        <v>4</v>
-      </c>
-      <c r="L69">
-        <v>108</v>
-      </c>
       <c r="M69">
         <v>4</v>
       </c>
@@ -13750,12 +13640,6 @@
       <c r="J70" t="s">
         <v>758</v>
       </c>
-      <c r="K70" t="s">
-        <v>4</v>
-      </c>
-      <c r="L70">
-        <v>108</v>
-      </c>
       <c r="M70">
         <v>5</v>
       </c>
@@ -13822,7 +13706,7 @@
         <v>4</v>
       </c>
       <c r="L71">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="M71">
         <v>8</v>
@@ -13890,7 +13774,7 @@
         <v>4</v>
       </c>
       <c r="L72">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="M72">
         <v>2</v>
@@ -13961,7 +13845,7 @@
         <v>4</v>
       </c>
       <c r="L73">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="M73">
         <v>1</v>
@@ -14105,12 +13989,6 @@
       <c r="J75" t="s">
         <v>758</v>
       </c>
-      <c r="K75" t="s">
-        <v>4</v>
-      </c>
-      <c r="L75">
-        <v>108</v>
-      </c>
       <c r="M75">
         <v>5</v>
       </c>
@@ -14161,12 +14039,6 @@
       <c r="J76" t="s">
         <v>758</v>
       </c>
-      <c r="K76" t="s">
-        <v>4</v>
-      </c>
-      <c r="L76">
-        <v>108</v>
-      </c>
       <c r="M76">
         <v>4</v>
       </c>
@@ -14208,12 +14080,6 @@
       <c r="J77" t="s">
         <v>758</v>
       </c>
-      <c r="K77" t="s">
-        <v>4</v>
-      </c>
-      <c r="L77">
-        <v>108</v>
-      </c>
       <c r="M77">
         <v>1</v>
       </c>
@@ -14255,12 +14121,6 @@
       <c r="J78" t="s">
         <v>758</v>
       </c>
-      <c r="K78" t="s">
-        <v>4</v>
-      </c>
-      <c r="L78">
-        <v>108</v>
-      </c>
       <c r="M78">
         <v>2</v>
       </c>
@@ -14311,12 +14171,6 @@
       <c r="J79" t="s">
         <v>758</v>
       </c>
-      <c r="K79" t="s">
-        <v>4</v>
-      </c>
-      <c r="L79">
-        <v>108</v>
-      </c>
       <c r="M79">
         <v>3</v>
       </c>
@@ -14513,7 +14367,7 @@
         <v>4</v>
       </c>
       <c r="L82">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M82">
         <v>3</v>
@@ -14587,7 +14441,7 @@
         <v>4</v>
       </c>
       <c r="L83">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="M83">
         <v>5</v>
@@ -14731,12 +14585,6 @@
       <c r="J85" t="s">
         <v>758</v>
       </c>
-      <c r="K85" t="s">
-        <v>4</v>
-      </c>
-      <c r="L85">
-        <v>109</v>
-      </c>
       <c r="M85">
         <v>3</v>
       </c>
@@ -14803,7 +14651,7 @@
         <v>4</v>
       </c>
       <c r="L86">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="M86">
         <v>2</v>
@@ -14852,12 +14700,6 @@
       <c r="J87" t="s">
         <v>758</v>
       </c>
-      <c r="K87" t="s">
-        <v>4</v>
-      </c>
-      <c r="L87">
-        <v>109</v>
-      </c>
       <c r="M87">
         <v>5</v>
       </c>
@@ -14905,12 +14747,6 @@
       <c r="J88" t="s">
         <v>758</v>
       </c>
-      <c r="K88" t="s">
-        <v>4</v>
-      </c>
-      <c r="L88">
-        <v>109</v>
-      </c>
       <c r="M88">
         <v>4</v>
       </c>
@@ -14956,7 +14792,7 @@
         <v>4</v>
       </c>
       <c r="L89">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M89">
         <v>1</v>
@@ -15129,12 +14965,6 @@
       <c r="J92" t="s">
         <v>758</v>
       </c>
-      <c r="K92" t="s">
-        <v>4</v>
-      </c>
-      <c r="L92">
-        <v>111</v>
-      </c>
       <c r="M92">
         <v>3</v>
       </c>
@@ -15204,7 +15034,7 @@
         <v>4</v>
       </c>
       <c r="L93">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="M93">
         <v>1</v>
@@ -15272,7 +15102,7 @@
         <v>4</v>
       </c>
       <c r="L94">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M94">
         <v>5</v>
@@ -15338,12 +15168,6 @@
       </c>
       <c r="J95" t="s">
         <v>758</v>
-      </c>
-      <c r="K95" t="s">
-        <v>4</v>
-      </c>
-      <c r="L95">
-        <v>111</v>
       </c>
       <c r="M95">
         <v>5</v>
@@ -15545,12 +15369,6 @@
       <c r="J98" t="s">
         <v>758</v>
       </c>
-      <c r="K98" t="s">
-        <v>4</v>
-      </c>
-      <c r="L98">
-        <v>111</v>
-      </c>
       <c r="M98">
         <v>3</v>
       </c>
@@ -15592,12 +15410,6 @@
       <c r="J99" t="s">
         <v>758</v>
       </c>
-      <c r="K99" t="s">
-        <v>4</v>
-      </c>
-      <c r="L99">
-        <v>111</v>
-      </c>
       <c r="M99">
         <v>5</v>
       </c>
@@ -15642,12 +15454,6 @@
       <c r="J100" t="s">
         <v>758</v>
       </c>
-      <c r="K100" t="s">
-        <v>4</v>
-      </c>
-      <c r="L100">
-        <v>111</v>
-      </c>
       <c r="M100">
         <v>2</v>
       </c>
@@ -15692,12 +15498,6 @@
       <c r="J101" t="s">
         <v>758</v>
       </c>
-      <c r="K101" t="s">
-        <v>4</v>
-      </c>
-      <c r="L101">
-        <v>112</v>
-      </c>
       <c r="M101">
         <v>5</v>
       </c>
@@ -15764,7 +15564,7 @@
         <v>4</v>
       </c>
       <c r="L102">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="M102">
         <v>2</v>
@@ -15832,7 +15632,7 @@
         <v>4</v>
       </c>
       <c r="L103">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M103">
         <v>1</v>
@@ -15974,7 +15774,7 @@
         <v>4</v>
       </c>
       <c r="L105">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="M105">
         <v>3</v>
@@ -16203,12 +16003,6 @@
       <c r="J109" t="s">
         <v>758</v>
       </c>
-      <c r="K109" t="s">
-        <v>4</v>
-      </c>
-      <c r="L109">
-        <v>112</v>
-      </c>
       <c r="M109">
         <v>4</v>
       </c>
@@ -16254,7 +16048,7 @@
         <v>4</v>
       </c>
       <c r="L110">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="M110">
         <v>2</v>
@@ -16303,12 +16097,6 @@
       <c r="J111" t="s">
         <v>758</v>
       </c>
-      <c r="K111" t="s">
-        <v>4</v>
-      </c>
-      <c r="L111">
-        <v>112</v>
-      </c>
       <c r="M111">
         <v>3</v>
       </c>
@@ -16425,7 +16213,7 @@
         <v>4</v>
       </c>
       <c r="L113">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="M113">
         <v>4</v>
@@ -16493,7 +16281,7 @@
         <v>4</v>
       </c>
       <c r="L114">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="M114">
         <v>5</v>
@@ -16561,7 +16349,7 @@
         <v>4</v>
       </c>
       <c r="L115">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="M115">
         <v>2</v>
@@ -16703,7 +16491,7 @@
         <v>4</v>
       </c>
       <c r="L117" s="1">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="M117" s="1">
         <v>1</v>
@@ -16780,12 +16568,6 @@
       <c r="J118" t="s">
         <v>758</v>
       </c>
-      <c r="K118" t="s">
-        <v>4</v>
-      </c>
-      <c r="L118">
-        <v>113</v>
-      </c>
       <c r="M118">
         <v>1</v>
       </c>
@@ -16827,12 +16609,6 @@
       <c r="J119" t="s">
         <v>758</v>
       </c>
-      <c r="K119" t="s">
-        <v>4</v>
-      </c>
-      <c r="L119">
-        <v>113</v>
-      </c>
       <c r="M119">
         <v>3</v>
       </c>
@@ -16934,7 +16710,7 @@
         <v>4</v>
       </c>
       <c r="L121">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M121">
         <v>4</v>
@@ -17218,7 +16994,7 @@
         <v>4</v>
       </c>
       <c r="L125" s="1">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M125" s="1">
         <v>2</v>
@@ -17298,12 +17074,6 @@
       <c r="J126" t="s">
         <v>758</v>
       </c>
-      <c r="K126" t="s">
-        <v>4</v>
-      </c>
-      <c r="L126">
-        <v>114</v>
-      </c>
       <c r="M126">
         <v>2</v>
       </c>
@@ -17351,12 +17121,6 @@
       <c r="J127" t="s">
         <v>758</v>
       </c>
-      <c r="K127" t="s">
-        <v>4</v>
-      </c>
-      <c r="L127">
-        <v>114</v>
-      </c>
       <c r="M127">
         <v>3</v>
       </c>
@@ -17404,12 +17168,6 @@
       <c r="J128" t="s">
         <v>758</v>
       </c>
-      <c r="K128" t="s">
-        <v>4</v>
-      </c>
-      <c r="L128">
-        <v>114</v>
-      </c>
       <c r="M128">
         <v>4</v>
       </c>
@@ -22258,10 +22016,10 @@
         <v>758</v>
       </c>
       <c r="K201" t="s">
-        <v>66</v>
+        <v>4</v>
       </c>
       <c r="L201">
-        <v>304</v>
+        <v>114</v>
       </c>
       <c r="M201">
         <v>4</v>
@@ -24443,10 +24201,10 @@
         <v>758</v>
       </c>
       <c r="K234" t="s">
-        <v>66</v>
+        <v>4</v>
       </c>
       <c r="L234">
-        <v>312</v>
+        <v>112</v>
       </c>
       <c r="M234">
         <v>3</v>
@@ -24582,10 +24340,10 @@
         <v>758</v>
       </c>
       <c r="K236" t="s">
-        <v>66</v>
+        <v>4</v>
       </c>
       <c r="L236">
-        <v>312</v>
+        <v>109</v>
       </c>
       <c r="M236">
         <v>5</v>
@@ -31129,8 +30887,11 @@
       <c r="I325" t="s">
         <v>761</v>
       </c>
+      <c r="K325" t="s">
+        <v>4</v>
+      </c>
       <c r="L325">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="M325">
         <v>3</v>
@@ -31198,8 +30959,11 @@
       <c r="I326" t="s">
         <v>765</v>
       </c>
+      <c r="K326" t="s">
+        <v>4</v>
+      </c>
       <c r="L326">
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="M326">
         <v>5</v>
@@ -36059,8 +35823,12 @@
       <c r="J405" s="1" t="s">
         <v>758</v>
       </c>
-      <c r="K405" s="1"/>
-      <c r="L405" s="1"/>
+      <c r="K405" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L405" s="1">
+        <v>107</v>
+      </c>
       <c r="M405" s="1">
         <v>3</v>
       </c>
@@ -36499,6 +36267,12 @@
       </c>
       <c r="J411" t="s">
         <v>758</v>
+      </c>
+      <c r="K411" t="s">
+        <v>4</v>
+      </c>
+      <c r="L411">
+        <v>104</v>
       </c>
       <c r="M411">
         <v>3</v>
@@ -37170,7 +36944,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>